<commit_message>
change lotsize to propertytype
</commit_message>
<xml_diff>
--- a/RawData/properties.xlsx
+++ b/RawData/properties.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/07d7b2bcce4ed218/Desktop/608-607Project/RawData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="119" documentId="11_F25DC773A252ABDACC1048ECB1DF455E5BDE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4151E9BD-4AE0-49C8-99D4-9D17B95A4A74}"/>
+  <xr:revisionPtr revIDLastSave="125" documentId="11_F25DC773A252ABDACC1048ECB1DF455E5BDE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7774AF1E-A4B6-43B0-AD95-4DFB083E5CCB}"/>
   <bookViews>
     <workbookView xWindow="2355" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1070,9 +1070,6 @@
     <t>11 Crocker Place, Winnipeg, MB</t>
   </si>
   <si>
-    <t>LotSize</t>
-  </si>
-  <si>
     <t>Bedrooms</t>
   </si>
   <si>
@@ -1092,6 +1089,9 @@
   </si>
   <si>
     <t>feras@ucalgary.ca</t>
+  </si>
+  <si>
+    <t>PropertyType</t>
   </si>
 </sst>
 </file>
@@ -1438,7 +1438,7 @@
   <dimension ref="A1:J188"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="J2" sqref="J2:J188"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1448,7 +1448,7 @@
     <col min="3" max="3" width="11.54296875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.1796875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8" customWidth="1"/>
+    <col min="6" max="6" width="12.26953125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.08984375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.453125" bestFit="1" customWidth="1"/>
   </cols>
@@ -1461,22 +1461,22 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>345</v>
+      </c>
+      <c r="D1" t="s">
+        <v>343</v>
+      </c>
+      <c r="E1" t="s">
+        <v>344</v>
+      </c>
+      <c r="F1" t="s">
+        <v>350</v>
+      </c>
+      <c r="G1" t="s">
         <v>346</v>
       </c>
-      <c r="D1" t="s">
-        <v>344</v>
-      </c>
-      <c r="E1" t="s">
-        <v>345</v>
-      </c>
-      <c r="F1" t="s">
-        <v>343</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>347</v>
-      </c>
-      <c r="H1" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
@@ -1495,18 +1495,19 @@
       <c r="E2">
         <v>2</v>
       </c>
-      <c r="F2">
-        <v>1744</v>
+      <c r="F2" t="str">
+        <f>IF(D2&lt;3, "Condo", "House")</f>
+        <v>House</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H2">
         <v>1</v>
       </c>
       <c r="J2" t="str">
-        <f>_xlfn.CONCAT("('",A2, "'", ", ", "'", B2, "'", ", ", C2, ", ", D2, ", ", E2, ", ", F2, ", ", "'", G2, "'", ", ", H2, ")", ",")</f>
-        <v>('SK913993', '207 Lehrer PLACE, Saskatoon, SK S7R 0L4', 669900, 3, 2, 1744, 'ardit@ucalgary.ca', 1),</v>
+        <f>_xlfn.CONCAT("('",A2, "'", ", ", "'", B2, "'", ", ", C2, ", ", D2, ", ", E2, ", ", "'", F2, "'", ", ", "'", G2, "'", ", ", H2, ")", ",")</f>
+        <v>('SK913993', '207 Lehrer PLACE, Saskatoon, SK S7R 0L4', 669900, 3, 2, 'House', 'ardit@ucalgary.ca', 1),</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
@@ -1525,18 +1526,19 @@
       <c r="E3">
         <v>3</v>
       </c>
-      <c r="F3">
-        <v>1470</v>
+      <c r="F3" t="str">
+        <f t="shared" ref="F3:F66" si="0">IF(D3&lt;3, "Condo", "House")</f>
+        <v>House</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H3">
         <v>2</v>
       </c>
       <c r="J3" t="str">
-        <f t="shared" ref="J3:J66" si="0">_xlfn.CONCAT("('",A3, "'", ", ", "'", B3, "'", ", ", C3, ", ", D3, ", ", E3, ", ", F3, ", ", "'", G3, "'", ", ", H3, ")", ",")</f>
-        <v>('SK914061', '3104 Ortona STREET, Saskatoon, SK S7M 3R4', 619900, 3, 3, 1470, 'ardit@ucalgary.ca', 2),</v>
+        <f t="shared" ref="J3:J66" si="1">_xlfn.CONCAT("('",A3, "'", ", ", "'", B3, "'", ", ", C3, ", ", D3, ", ", E3, ", ", "'", F3, "'", ", ", "'", G3, "'", ", ", H3, ")", ",")</f>
+        <v>('SK914061', '3104 Ortona STREET, Saskatoon, SK S7M 3R4', 619900, 3, 3, 'House', 'ardit@ucalgary.ca', 2),</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
@@ -1555,18 +1557,19 @@
       <c r="E4">
         <v>3</v>
       </c>
-      <c r="F4">
-        <v>1290</v>
+      <c r="F4" t="str">
+        <f t="shared" si="0"/>
+        <v>House</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H4">
         <v>3</v>
       </c>
       <c r="J4" t="str">
-        <f t="shared" si="0"/>
-        <v>('SK914153', '714A Victoria AVENUE, Saskatoon, SK S7N 0Z2', 374900, 3, 3, 1290, 'ardit@ucalgary.ca', 3),</v>
+        <f t="shared" si="1"/>
+        <v>('SK914153', '714A Victoria AVENUE, Saskatoon, SK S7N 0Z2', 374900, 3, 3, 'House', 'ardit@ucalgary.ca', 3),</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
@@ -1585,18 +1588,19 @@
       <c r="E5">
         <v>3</v>
       </c>
-      <c r="F5">
-        <v>1953</v>
+      <c r="F5" t="str">
+        <f t="shared" si="0"/>
+        <v>House</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H5">
         <v>1</v>
       </c>
       <c r="J5" t="str">
-        <f t="shared" si="0"/>
-        <v>('SK914148', '246 Frobisher CRESCENT, Saskatoon, SK S7K 4Y7', 479900, 5, 3, 1953, 'ardit@ucalgary.ca', 1),</v>
+        <f t="shared" si="1"/>
+        <v>('SK914148', '246 Frobisher CRESCENT, Saskatoon, SK S7K 4Y7', 479900, 5, 3, 'House', 'ardit@ucalgary.ca', 1),</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
@@ -1615,18 +1619,19 @@
       <c r="E6">
         <v>3</v>
       </c>
-      <c r="F6">
-        <v>1837</v>
+      <c r="F6" t="str">
+        <f t="shared" si="0"/>
+        <v>House</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H6">
         <v>2</v>
       </c>
       <c r="J6" t="str">
-        <f t="shared" si="0"/>
-        <v>('SK914086', '739 Hastings COVE, Saskatoon, SK S7V 0G6', 899900, 4, 3, 1837, 'ardit@ucalgary.ca', 2),</v>
+        <f t="shared" si="1"/>
+        <v>('SK914086', '739 Hastings COVE, Saskatoon, SK S7V 0G6', 899900, 4, 3, 'House', 'ardit@ucalgary.ca', 2),</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
@@ -1645,18 +1650,19 @@
       <c r="E7">
         <v>3</v>
       </c>
-      <c r="F7">
-        <v>1295</v>
+      <c r="F7" t="str">
+        <f t="shared" si="0"/>
+        <v>House</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H7">
         <v>3</v>
       </c>
       <c r="J7" t="str">
-        <f t="shared" si="0"/>
-        <v>('SK914075', '334 Crean CRESCENT, Saskatoon, SK S7J 3X2', 419900, 4, 3, 1295, 'ardit@ucalgary.ca', 3),</v>
+        <f t="shared" si="1"/>
+        <v>('SK914075', '334 Crean CRESCENT, Saskatoon, SK S7J 3X2', 419900, 4, 3, 'House', 'ardit@ucalgary.ca', 3),</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
@@ -1675,18 +1681,19 @@
       <c r="E8">
         <v>3</v>
       </c>
-      <c r="F8">
-        <v>1574</v>
+      <c r="F8" t="str">
+        <f t="shared" si="0"/>
+        <v>House</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H8">
         <v>1</v>
       </c>
       <c r="J8" t="str">
-        <f t="shared" si="0"/>
-        <v>('SK914144', '962 Kloppenburg CRESCENT, Saskatoon, SK S7W 0P2', 559900, 5, 3, 1574, 'ardit@ucalgary.ca', 1),</v>
+        <f t="shared" si="1"/>
+        <v>('SK914144', '962 Kloppenburg CRESCENT, Saskatoon, SK S7W 0P2', 559900, 5, 3, 'House', 'ardit@ucalgary.ca', 1),</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
@@ -1705,18 +1712,19 @@
       <c r="E9">
         <v>3</v>
       </c>
-      <c r="F9">
-        <v>1737</v>
+      <c r="F9" t="str">
+        <f t="shared" si="0"/>
+        <v>House</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H9">
         <v>2</v>
       </c>
       <c r="J9" t="str">
-        <f t="shared" si="0"/>
-        <v>('SK914082', '2435 Rosewood DRIVE, Saskatoon, SK S7V 0Z3', 554300, 3, 3, 1737, 'ardit@ucalgary.ca', 2),</v>
+        <f t="shared" si="1"/>
+        <v>('SK914082', '2435 Rosewood DRIVE, Saskatoon, SK S7V 0Z3', 554300, 3, 3, 'House', 'ardit@ucalgary.ca', 2),</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
@@ -1735,18 +1743,19 @@
       <c r="E10">
         <v>3</v>
       </c>
-      <c r="F10">
-        <v>1136</v>
+      <c r="F10" t="str">
+        <f t="shared" si="0"/>
+        <v>House</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H10">
         <v>3</v>
       </c>
       <c r="J10" t="str">
-        <f t="shared" si="0"/>
-        <v>('SK914108', '1 Bow COURT, Saskatoon, SK S7K 1H9', 399000, 4, 3, 1136, 'ardit@ucalgary.ca', 3),</v>
+        <f t="shared" si="1"/>
+        <v>('SK914108', '1 Bow COURT, Saskatoon, SK S7K 1H9', 399000, 4, 3, 'House', 'ardit@ucalgary.ca', 3),</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
@@ -1765,18 +1774,19 @@
       <c r="E11">
         <v>2</v>
       </c>
-      <c r="F11">
-        <v>1513</v>
+      <c r="F11" t="str">
+        <f t="shared" si="0"/>
+        <v>House</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H11">
         <v>1</v>
       </c>
       <c r="J11" t="str">
-        <f t="shared" si="0"/>
-        <v>('E4320360', '14611 95th St NW, Edmonton, AB T5E 3Y7', 575000, 6, 2, 1513, 'ardit@ucalgary.ca', 1),</v>
+        <f t="shared" si="1"/>
+        <v>('E4320360', '14611 95th St NW, Edmonton, AB T5E 3Y7', 575000, 6, 2, 'House', 'ardit@ucalgary.ca', 1),</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
@@ -1795,18 +1805,19 @@
       <c r="E12">
         <v>3</v>
       </c>
-      <c r="F12">
-        <v>1215</v>
+      <c r="F12" t="str">
+        <f t="shared" si="0"/>
+        <v>Condo</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H12">
         <v>2</v>
       </c>
       <c r="J12" t="str">
-        <f t="shared" si="0"/>
-        <v>('E4320364', '10465 42nd Ave NW, Edmonton, AB T6J 7C7', 429900, 2, 3, 1215, 'ardit@ucalgary.ca', 2),</v>
+        <f t="shared" si="1"/>
+        <v>('E4320364', '10465 42nd Ave NW, Edmonton, AB T6J 7C7', 429900, 2, 3, 'Condo', 'ardit@ucalgary.ca', 2),</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
@@ -1825,18 +1836,19 @@
       <c r="E13">
         <v>2</v>
       </c>
-      <c r="F13">
-        <v>1387</v>
+      <c r="F13" t="str">
+        <f t="shared" si="0"/>
+        <v>House</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H13">
         <v>3</v>
       </c>
       <c r="J13" t="str">
-        <f t="shared" si="0"/>
-        <v>('E4320358', '10346 142nd St NW, Edmonton, AB T5N 2P1', 393000, 5, 2, 1387, 'ardit@ucalgary.ca', 3),</v>
+        <f t="shared" si="1"/>
+        <v>('E4320358', '10346 142nd St NW, Edmonton, AB T5N 2P1', 393000, 5, 2, 'House', 'ardit@ucalgary.ca', 3),</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
@@ -1855,18 +1867,19 @@
       <c r="E14">
         <v>3</v>
       </c>
-      <c r="F14">
-        <v>1019</v>
+      <c r="F14" t="str">
+        <f t="shared" si="0"/>
+        <v>House</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H14">
         <v>1</v>
       </c>
       <c r="J14" t="str">
-        <f t="shared" si="0"/>
-        <v>('E4320355', '5512 145th Ave NW, Edmonton, AB T5A 3R3', 185000, 3, 3, 1019, 'ardit@ucalgary.ca', 1),</v>
+        <f t="shared" si="1"/>
+        <v>('E4320355', '5512 145th Ave NW, Edmonton, AB T5A 3R3', 185000, 3, 3, 'House', 'ardit@ucalgary.ca', 1),</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
@@ -1885,18 +1898,19 @@
       <c r="E15">
         <v>3</v>
       </c>
-      <c r="F15">
-        <v>1475</v>
+      <c r="F15" t="str">
+        <f t="shared" si="0"/>
+        <v>House</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H15">
         <v>2</v>
       </c>
       <c r="J15" t="str">
-        <f t="shared" si="0"/>
-        <v>('E4320309', '4611 128th Ave NW, Edmonton, AB T5A 2M7', 399900, 4, 3, 1475, 'ardit@ucalgary.ca', 2),</v>
+        <f t="shared" si="1"/>
+        <v>('E4320309', '4611 128th Ave NW, Edmonton, AB T5A 2M7', 399900, 4, 3, 'House', 'ardit@ucalgary.ca', 2),</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
@@ -1915,18 +1929,19 @@
       <c r="E16">
         <v>1</v>
       </c>
-      <c r="F16">
-        <v>631</v>
+      <c r="F16" t="str">
+        <f t="shared" si="0"/>
+        <v>Condo</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H16">
         <v>3</v>
       </c>
       <c r="J16" t="str">
-        <f t="shared" si="0"/>
-        <v>('E4320357', '7339 S Terwillegar Dr NW #1418, Edmonton, AB T6R 0M1', 130000, 1, 1, 631, 'ardit@ucalgary.ca', 3),</v>
+        <f t="shared" si="1"/>
+        <v>('E4320357', '7339 S Terwillegar Dr NW #1418, Edmonton, AB T6R 0M1', 130000, 1, 1, 'Condo', 'ardit@ucalgary.ca', 3),</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.35">
@@ -1945,18 +1960,19 @@
       <c r="E17">
         <v>4</v>
       </c>
-      <c r="F17">
-        <v>2161</v>
+      <c r="F17" t="str">
+        <f t="shared" si="0"/>
+        <v>House</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H17">
         <v>1</v>
       </c>
       <c r="J17" t="str">
-        <f t="shared" si="0"/>
-        <v>('E4320331', '1711 109th St NW, Edmonton, AB T6J 5Z8', 519900, 5, 4, 2161, 'ardit@ucalgary.ca', 1),</v>
+        <f t="shared" si="1"/>
+        <v>('E4320331', '1711 109th St NW, Edmonton, AB T6J 5Z8', 519900, 5, 4, 'House', 'ardit@ucalgary.ca', 1),</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.35">
@@ -1975,18 +1991,19 @@
       <c r="E18">
         <v>2</v>
       </c>
-      <c r="F18">
-        <v>1072</v>
+      <c r="F18" t="str">
+        <f t="shared" si="0"/>
+        <v>House</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H18">
         <v>2</v>
       </c>
       <c r="J18" t="str">
-        <f t="shared" si="0"/>
-        <v>('E4320291', '13239 Delwood Rd NW, Edmonton, AB T5C 3B5', 299990, 5, 2, 1072, 'ardit@ucalgary.ca', 2),</v>
+        <f t="shared" si="1"/>
+        <v>('E4320291', '13239 Delwood Rd NW, Edmonton, AB T5C 3B5', 299990, 5, 2, 'House', 'ardit@ucalgary.ca', 2),</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.35">
@@ -2005,18 +2022,19 @@
       <c r="E19">
         <v>3</v>
       </c>
-      <c r="F19">
-        <v>1083</v>
+      <c r="F19" t="str">
+        <f t="shared" si="0"/>
+        <v>House</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H19">
         <v>3</v>
       </c>
       <c r="J19" t="str">
-        <f t="shared" si="0"/>
-        <v>('E4320295', '12631 161st Ave NW, Edmonton, AB T5X 4W7', 350000, 4, 3, 1083, 'ardit@ucalgary.ca', 3),</v>
+        <f t="shared" si="1"/>
+        <v>('E4320295', '12631 161st Ave NW, Edmonton, AB T5X 4W7', 350000, 4, 3, 'House', 'ardit@ucalgary.ca', 3),</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.35">
@@ -2035,18 +2053,19 @@
       <c r="E20">
         <v>3</v>
       </c>
-      <c r="F20">
-        <v>1620</v>
+      <c r="F20" t="str">
+        <f t="shared" si="0"/>
+        <v>House</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H20">
         <v>1</v>
       </c>
       <c r="J20" t="str">
-        <f t="shared" si="0"/>
-        <v>('C4320250', '64 S Citadel Dr NW, Calgary, AB T3G 3V1', 529900, 3, 3, 1620, 'ardit@ucalgary.ca', 1),</v>
+        <f t="shared" si="1"/>
+        <v>('C4320250', '64 S Citadel Dr NW, Calgary, AB T3G 3V1', 529900, 3, 3, 'House', 'ardit@ucalgary.ca', 1),</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.35">
@@ -2065,18 +2084,19 @@
       <c r="E21">
         <v>3</v>
       </c>
-      <c r="F21">
-        <v>1223</v>
+      <c r="F21" t="str">
+        <f t="shared" si="0"/>
+        <v>House</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H21">
         <v>2</v>
       </c>
       <c r="J21" t="str">
-        <f t="shared" si="0"/>
-        <v>('C4320251', '957 S Rundlecairn Way NE, Calgary, AB T1Y 2W7', 429900, 5, 3, 1223, 'ardit@ucalgary.ca', 2),</v>
+        <f t="shared" si="1"/>
+        <v>('C4320251', '957 S Rundlecairn Way NE, Calgary, AB T1Y 2W7', 429900, 5, 3, 'House', 'ardit@ucalgary.ca', 2),</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.35">
@@ -2095,18 +2115,19 @@
       <c r="E22">
         <v>3</v>
       </c>
-      <c r="F22">
-        <v>1210</v>
+      <c r="F22" t="str">
+        <f t="shared" si="0"/>
+        <v>House</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H22">
         <v>3</v>
       </c>
       <c r="J22" t="str">
-        <f t="shared" si="0"/>
-        <v>('C4320252', '220 W Deer Park Pl SE, Calgary, AB T2J 5M2', 499900, 4, 3, 1210, 'ardit@ucalgary.ca', 3),</v>
+        <f t="shared" si="1"/>
+        <v>('C4320252', '220 W Deer Park Pl SE, Calgary, AB T2J 5M2', 499900, 4, 3, 'House', 'ardit@ucalgary.ca', 3),</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.35">
@@ -2125,18 +2146,19 @@
       <c r="E23">
         <v>2</v>
       </c>
-      <c r="F23">
-        <v>850</v>
+      <c r="F23" t="str">
+        <f t="shared" si="0"/>
+        <v>Condo</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H23">
         <v>1</v>
       </c>
       <c r="J23" t="str">
-        <f t="shared" si="0"/>
-        <v>('C4320253', '10 Sage Hill Way NW #111, Calgary, AB T3R 0H5', 369900, 2, 2, 850, 'ardit@ucalgary.ca', 1),</v>
+        <f t="shared" si="1"/>
+        <v>('C4320253', '10 Sage Hill Way NW #111, Calgary, AB T3R 0H5', 369900, 2, 2, 'Condo', 'ardit@ucalgary.ca', 1),</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.35">
@@ -2155,18 +2177,19 @@
       <c r="E24">
         <v>3</v>
       </c>
-      <c r="F24">
-        <v>1858</v>
+      <c r="F24" t="str">
+        <f t="shared" si="0"/>
+        <v>House</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H24">
         <v>2</v>
       </c>
       <c r="J24" t="str">
-        <f t="shared" si="0"/>
-        <v>('C4320254', '425 N 12th Ave NE, Calgary, AB T2E 1A7', 799500, 4, 3, 1858, 'ardit@ucalgary.ca', 2),</v>
+        <f t="shared" si="1"/>
+        <v>('C4320254', '425 N 12th Ave NE, Calgary, AB T2E 1A7', 799500, 4, 3, 'House', 'ardit@ucalgary.ca', 2),</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.35">
@@ -2185,18 +2208,19 @@
       <c r="E25">
         <v>1</v>
       </c>
-      <c r="F25">
-        <v>815</v>
+      <c r="F25" t="str">
+        <f t="shared" si="0"/>
+        <v>Condo</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H25">
         <v>3</v>
       </c>
       <c r="J25" t="str">
-        <f t="shared" si="0"/>
-        <v>('C4320255', '3519 N 49th St NW #28, Calgary, AB T3A 2C7', 189000, 2, 1, 815, 'ardit@ucalgary.ca', 3),</v>
+        <f t="shared" si="1"/>
+        <v>('C4320255', '3519 N 49th St NW #28, Calgary, AB T3A 2C7', 189000, 2, 1, 'Condo', 'ardit@ucalgary.ca', 3),</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.35">
@@ -2215,18 +2239,19 @@
       <c r="E26">
         <v>3</v>
       </c>
-      <c r="F26">
-        <v>1448</v>
+      <c r="F26" t="str">
+        <f t="shared" si="0"/>
+        <v>House</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H26">
         <v>1</v>
       </c>
       <c r="J26" t="str">
-        <f t="shared" si="0"/>
-        <v>('C4320256', '2232 Langriville Dr SW, Calgary, AB T3E 5G7', 925000, 5, 3, 1448, 'ardit@ucalgary.ca', 1),</v>
+        <f t="shared" si="1"/>
+        <v>('C4320256', '2232 Langriville Dr SW, Calgary, AB T3E 5G7', 925000, 5, 3, 'House', 'ardit@ucalgary.ca', 1),</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.35">
@@ -2245,18 +2270,19 @@
       <c r="E27">
         <v>3</v>
       </c>
-      <c r="F27">
-        <v>2709</v>
+      <c r="F27" t="str">
+        <f t="shared" si="0"/>
+        <v>House</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H27">
         <v>2</v>
       </c>
       <c r="J27" t="str">
-        <f t="shared" si="0"/>
-        <v>('C4320257', '256 E Edgebank Cir NW, Calgary, AB T3A 4W1', 968000, 5, 3, 2709, 'ardit@ucalgary.ca', 2),</v>
+        <f t="shared" si="1"/>
+        <v>('C4320257', '256 E Edgebank Cir NW, Calgary, AB T3A 4W1', 968000, 5, 3, 'House', 'ardit@ucalgary.ca', 2),</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.35">
@@ -2275,18 +2301,19 @@
       <c r="E28">
         <v>2</v>
       </c>
-      <c r="F28">
-        <v>1905</v>
+      <c r="F28" t="str">
+        <f t="shared" si="0"/>
+        <v>House</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H28">
         <v>3</v>
       </c>
       <c r="J28" t="str">
-        <f t="shared" si="0"/>
-        <v>('C4320258', '3415 NE Bonita Cres NW, Calgary, AB T3B 2R9', 499000, 8, 2, 1905, 'ardit@ucalgary.ca', 3),</v>
+        <f t="shared" si="1"/>
+        <v>('C4320258', '3415 NE Bonita Cres NW, Calgary, AB T3B 2R9', 499000, 8, 2, 'House', 'ardit@ucalgary.ca', 3),</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.35">
@@ -2305,18 +2332,19 @@
       <c r="E29">
         <v>4</v>
       </c>
-      <c r="F29">
-        <v>0</v>
+      <c r="F29" t="str">
+        <f t="shared" si="0"/>
+        <v>House</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H29">
         <v>1</v>
       </c>
       <c r="J29" t="str">
-        <f t="shared" si="0"/>
-        <v>('W5827624', '173 Wallace Ave, Toronto, ON M6H 1V3', 1699000, 4, 4, 0, 'ardit@ucalgary.ca', 1),</v>
+        <f t="shared" si="1"/>
+        <v>('W5827624', '173 Wallace Ave, Toronto, ON M6H 1V3', 1699000, 4, 4, 'House', 'ardit@ucalgary.ca', 1),</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.35">
@@ -2335,18 +2363,19 @@
       <c r="E30">
         <v>2</v>
       </c>
-      <c r="F30">
-        <v>0</v>
+      <c r="F30" t="str">
+        <f t="shared" si="0"/>
+        <v>House</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H30">
         <v>2</v>
       </c>
       <c r="J30" t="str">
-        <f t="shared" si="0"/>
-        <v>('C5827688', '131 Hillmount Ave, Toronto, ON M6B 1X7', 1999000, 3, 2, 0, 'ardit@ucalgary.ca', 2),</v>
+        <f t="shared" si="1"/>
+        <v>('C5827688', '131 Hillmount Ave, Toronto, ON M6B 1X7', 1999000, 3, 2, 'House', 'ardit@ucalgary.ca', 2),</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.35">
@@ -2365,18 +2394,19 @@
       <c r="E31">
         <v>2</v>
       </c>
-      <c r="F31">
-        <v>0</v>
+      <c r="F31" t="str">
+        <f t="shared" si="0"/>
+        <v>House</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H31">
         <v>3</v>
       </c>
       <c r="J31" t="str">
-        <f t="shared" si="0"/>
-        <v>('E5827522', '1125 Warden Ave, Toronto, ON M1R 2P8', 1069000, 3, 2, 0, 'ardit@ucalgary.ca', 3),</v>
+        <f t="shared" si="1"/>
+        <v>('E5827522', '1125 Warden Ave, Toronto, ON M1R 2P8', 1069000, 3, 2, 'House', 'ardit@ucalgary.ca', 3),</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.35">
@@ -2395,18 +2425,19 @@
       <c r="E32">
         <v>1</v>
       </c>
-      <c r="F32">
-        <v>0</v>
+      <c r="F32" t="str">
+        <f t="shared" si="0"/>
+        <v>Condo</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H32">
         <v>1</v>
       </c>
       <c r="J32" t="str">
-        <f t="shared" si="0"/>
-        <v>('E5827792', '30 Baseball Pl #1408, Toronto, ON M4M 0E8', 539900, 1, 1, 0, 'ardit@ucalgary.ca', 1),</v>
+        <f t="shared" si="1"/>
+        <v>('E5827792', '30 Baseball Pl #1408, Toronto, ON M4M 0E8', 539900, 1, 1, 'Condo', 'ardit@ucalgary.ca', 1),</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.35">
@@ -2425,18 +2456,19 @@
       <c r="E33">
         <v>4</v>
       </c>
-      <c r="F33">
-        <v>0</v>
+      <c r="F33" t="str">
+        <f t="shared" si="0"/>
+        <v>House</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H33">
         <v>2</v>
       </c>
       <c r="J33" t="str">
-        <f t="shared" si="0"/>
-        <v>('E5827793', '51 Burnfield Ave, Toronto, ON M6G 1Y4', 2350000, 3, 4, 0, 'ardit@ucalgary.ca', 2),</v>
+        <f t="shared" si="1"/>
+        <v>('E5827793', '51 Burnfield Ave, Toronto, ON M6G 1Y4', 2350000, 3, 4, 'House', 'ardit@ucalgary.ca', 2),</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.35">
@@ -2455,18 +2487,19 @@
       <c r="E34">
         <v>1</v>
       </c>
-      <c r="F34">
-        <v>0</v>
+      <c r="F34" t="str">
+        <f t="shared" si="0"/>
+        <v>Condo</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H34">
         <v>3</v>
       </c>
       <c r="J34" t="str">
-        <f t="shared" si="0"/>
-        <v>('E5827794', '55 Harbour Sq #2516, Toronto, ON M5J 2L1', 698000, 1, 1, 0, 'ardit@ucalgary.ca', 3),</v>
+        <f t="shared" si="1"/>
+        <v>('E5827794', '55 Harbour Sq #2516, Toronto, ON M5J 2L1', 698000, 1, 1, 'Condo', 'ardit@ucalgary.ca', 3),</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.35">
@@ -2485,18 +2518,19 @@
       <c r="E35">
         <v>2</v>
       </c>
-      <c r="F35">
-        <v>0</v>
+      <c r="F35" t="str">
+        <f t="shared" si="0"/>
+        <v>House</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H35">
         <v>1</v>
       </c>
       <c r="J35" t="str">
-        <f t="shared" si="0"/>
-        <v>('C5827824', '45 Sunrise Ave #104, Toronto, ON M4A 2S3', 599999, 3, 2, 0, 'ardit@ucalgary.ca', 1),</v>
+        <f t="shared" si="1"/>
+        <v>('C5827824', '45 Sunrise Ave #104, Toronto, ON M4A 2S3', 599999, 3, 2, 'House', 'ardit@ucalgary.ca', 1),</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.35">
@@ -2515,18 +2549,19 @@
       <c r="E36">
         <v>4</v>
       </c>
-      <c r="F36">
-        <v>0</v>
+      <c r="F36" t="str">
+        <f t="shared" si="0"/>
+        <v>House</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H36">
         <v>2</v>
       </c>
       <c r="J36" t="str">
-        <f t="shared" si="0"/>
-        <v>('C5827723', '348 Brunswick Ave, Toronto, ON M5R 2Y9', 2995000, 4, 4, 0, 'ardit@ucalgary.ca', 2),</v>
+        <f t="shared" si="1"/>
+        <v>('C5827723', '348 Brunswick Ave, Toronto, ON M5R 2Y9', 2995000, 4, 4, 'House', 'ardit@ucalgary.ca', 2),</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.35">
@@ -2545,18 +2580,19 @@
       <c r="E37">
         <v>2</v>
       </c>
-      <c r="F37">
-        <v>0</v>
+      <c r="F37" t="str">
+        <f t="shared" si="0"/>
+        <v>Condo</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H37">
         <v>3</v>
       </c>
       <c r="J37" t="str">
-        <f t="shared" si="0"/>
-        <v>('C5827831', '33 Bay St #2808, Toronto, ON M5J 2Z3', 1258000, 2, 2, 0, 'ardit@ucalgary.ca', 3),</v>
+        <f t="shared" si="1"/>
+        <v>('C5827831', '33 Bay St #2808, Toronto, ON M5J 2Z3', 1258000, 2, 2, 'Condo', 'ardit@ucalgary.ca', 3),</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.35">
@@ -2575,18 +2611,19 @@
       <c r="E38">
         <v>3</v>
       </c>
-      <c r="F38">
-        <v>0</v>
+      <c r="F38" t="str">
+        <f t="shared" si="0"/>
+        <v>House</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H38">
         <v>1</v>
       </c>
       <c r="J38" t="str">
-        <f t="shared" si="0"/>
-        <v>('W5827705', '485 Meadows Blvd #12, Mississauga, ON L4Z 1H1', 824900, 3, 3, 0, 'ardit@ucalgary.ca', 1),</v>
+        <f t="shared" si="1"/>
+        <v>('W5827705', '485 Meadows Blvd #12, Mississauga, ON L4Z 1H1', 824900, 3, 3, 'House', 'ardit@ucalgary.ca', 1),</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.35">
@@ -2605,18 +2642,19 @@
       <c r="E39">
         <v>2</v>
       </c>
-      <c r="F39">
-        <v>0</v>
+      <c r="F39" t="str">
+        <f t="shared" si="0"/>
+        <v>Condo</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H39">
         <v>2</v>
       </c>
       <c r="J39" t="str">
-        <f t="shared" si="0"/>
-        <v>('W5827706', '2929 Aquitaine Ave #405, Mississauga, ON L5N 2C7', 500000, 2, 2, 0, 'ardit@ucalgary.ca', 2),</v>
+        <f t="shared" si="1"/>
+        <v>('W5827706', '2929 Aquitaine Ave #405, Mississauga, ON L5N 2C7', 500000, 2, 2, 'Condo', 'ardit@ucalgary.ca', 2),</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.35">
@@ -2635,18 +2673,19 @@
       <c r="E40">
         <v>3</v>
       </c>
-      <c r="F40">
-        <v>0</v>
+      <c r="F40" t="str">
+        <f t="shared" si="0"/>
+        <v>House</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H40">
         <v>3</v>
       </c>
       <c r="J40" t="str">
-        <f t="shared" si="0"/>
-        <v>('W5827674', '6860 Glen Erin Dr UNIT 30, Mississauga, ON L5N 2E1', 789900, 3, 3, 0, 'ardit@ucalgary.ca', 3),</v>
+        <f t="shared" si="1"/>
+        <v>('W5827674', '6860 Glen Erin Dr UNIT 30, Mississauga, ON L5N 2E1', 789900, 3, 3, 'House', 'ardit@ucalgary.ca', 3),</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.35">
@@ -2665,18 +2704,19 @@
       <c r="E41">
         <v>2</v>
       </c>
-      <c r="F41">
-        <v>0</v>
+      <c r="F41" t="str">
+        <f t="shared" si="0"/>
+        <v>Condo</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H41">
         <v>1</v>
       </c>
       <c r="J41" t="str">
-        <f t="shared" si="0"/>
-        <v>('W5827547', '325 Webb Dr #310, Mississauga, ON L5B 3Z9', 549999, 2, 2, 0, 'ardit@ucalgary.ca', 1),</v>
+        <f t="shared" si="1"/>
+        <v>('W5827547', '325 Webb Dr #310, Mississauga, ON L5B 3Z9', 549999, 2, 2, 'Condo', 'ardit@ucalgary.ca', 1),</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.35">
@@ -2695,18 +2735,19 @@
       <c r="E42">
         <v>5</v>
       </c>
-      <c r="F42">
-        <v>0</v>
+      <c r="F42" t="str">
+        <f t="shared" si="0"/>
+        <v>House</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H42">
         <v>2</v>
       </c>
       <c r="J42" t="str">
-        <f t="shared" si="0"/>
-        <v>('W5827548', '1425 Chriseden Dr, Mississauga, ON L5H 1V3', 4125000, 4, 5, 0, 'ardit@ucalgary.ca', 2),</v>
+        <f t="shared" si="1"/>
+        <v>('W5827548', '1425 Chriseden Dr, Mississauga, ON L5H 1V3', 4125000, 4, 5, 'House', 'ardit@ucalgary.ca', 2),</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.35">
@@ -2725,18 +2766,19 @@
       <c r="E43">
         <v>3</v>
       </c>
-      <c r="F43">
-        <v>0</v>
+      <c r="F43" t="str">
+        <f t="shared" si="0"/>
+        <v>House</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H43">
         <v>3</v>
       </c>
       <c r="J43" t="str">
-        <f t="shared" si="0"/>
-        <v>('W5827299', '660 Arbor Rd, Mississauga, ON L5G 2J9', 999000, 4, 3, 0, 'ardit@ucalgary.ca', 3),</v>
+        <f t="shared" si="1"/>
+        <v>('W5827299', '660 Arbor Rd, Mississauga, ON L5G 2J9', 999000, 4, 3, 'House', 'ardit@ucalgary.ca', 3),</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.35">
@@ -2755,18 +2797,19 @@
       <c r="E44">
         <v>1</v>
       </c>
-      <c r="F44">
-        <v>0</v>
+      <c r="F44" t="str">
+        <f t="shared" si="0"/>
+        <v>House</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H44">
         <v>1</v>
       </c>
       <c r="J44" t="str">
-        <f t="shared" si="0"/>
-        <v>('W5827300', '945 Meadow Wood Rd, Mississauga, ON L5J 2S8', 2650000, 4, 1, 0, 'ardit@ucalgary.ca', 1),</v>
+        <f t="shared" si="1"/>
+        <v>('W5827300', '945 Meadow Wood Rd, Mississauga, ON L5J 2S8', 2650000, 4, 1, 'House', 'ardit@ucalgary.ca', 1),</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.35">
@@ -2785,18 +2828,19 @@
       <c r="E45">
         <v>3</v>
       </c>
-      <c r="F45">
-        <v>0</v>
+      <c r="F45" t="str">
+        <f t="shared" si="0"/>
+        <v>House</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H45">
         <v>2</v>
       </c>
       <c r="J45" t="str">
-        <f t="shared" si="0"/>
-        <v>('W5826773', '2358 Cobbinshaw Cir, Mississauga, ON L5N 2G3', 1089000, 3, 3, 0, 'ardit@ucalgary.ca', 2),</v>
+        <f t="shared" si="1"/>
+        <v>('W5826773', '2358 Cobbinshaw Cir, Mississauga, ON L5N 2G3', 1089000, 3, 3, 'House', 'ardit@ucalgary.ca', 2),</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.35">
@@ -2815,18 +2859,19 @@
       <c r="E46">
         <v>9</v>
       </c>
-      <c r="F46">
-        <v>8138</v>
+      <c r="F46" t="str">
+        <f t="shared" si="0"/>
+        <v>House</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H46">
         <v>3</v>
       </c>
       <c r="J46" t="str">
-        <f t="shared" si="0"/>
-        <v>('40331876', '2280 Doulton Dr, Mississauga, ON L5H 3M1', 13890000, 5, 9, 8138, 'ardit@ucalgary.ca', 3),</v>
+        <f t="shared" si="1"/>
+        <v>('40331876', '2280 Doulton Dr, Mississauga, ON L5H 3M1', 13890000, 5, 9, 'House', 'ardit@ucalgary.ca', 3),</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.35">
@@ -2845,18 +2890,19 @@
       <c r="E47">
         <v>2</v>
       </c>
-      <c r="F47">
-        <v>1724</v>
+      <c r="F47" t="str">
+        <f t="shared" si="0"/>
+        <v>House</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H47">
         <v>1</v>
       </c>
       <c r="J47" t="str">
-        <f t="shared" si="0"/>
-        <v>('202226140', '25 Remington Ct, Halifax, NS B3M 3Y6', 499900, 3, 2, 1724, 'ardit@ucalgary.ca', 1),</v>
+        <f t="shared" si="1"/>
+        <v>('202226140', '25 Remington Ct, Halifax, NS B3M 3Y6', 499900, 3, 2, 'House', 'ardit@ucalgary.ca', 1),</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.35">
@@ -2875,18 +2921,19 @@
       <c r="E48">
         <v>2</v>
       </c>
-      <c r="F48">
-        <v>1886</v>
+      <c r="F48" t="str">
+        <f t="shared" si="0"/>
+        <v>Condo</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H48">
         <v>2</v>
       </c>
       <c r="J48" t="str">
-        <f t="shared" si="0"/>
-        <v>('202225990', '55 Kearney Lake Rd, Halifax, NS B3M 2S6', 569900, 2, 2, 1886, 'ardit@ucalgary.ca', 2),</v>
+        <f t="shared" si="1"/>
+        <v>('202225990', '55 Kearney Lake Rd, Halifax, NS B3M 2S6', 569900, 2, 2, 'Condo', 'ardit@ucalgary.ca', 2),</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.35">
@@ -2905,18 +2952,19 @@
       <c r="E49">
         <v>5</v>
       </c>
-      <c r="F49">
-        <v>5550</v>
+      <c r="F49" t="str">
+        <f t="shared" si="0"/>
+        <v>House</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H49">
         <v>3</v>
       </c>
       <c r="J49" t="str">
-        <f t="shared" si="0"/>
-        <v>('202215459', '1160 Rockcliffe St, Halifax, NS B3H 3Y6', 7450000, 4, 5, 5550, 'ardit@ucalgary.ca', 3),</v>
+        <f t="shared" si="1"/>
+        <v>('202215459', '1160 Rockcliffe St, Halifax, NS B3H 3Y6', 7450000, 4, 5, 'House', 'ardit@ucalgary.ca', 3),</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.35">
@@ -2935,18 +2983,19 @@
       <c r="E50">
         <v>2</v>
       </c>
-      <c r="F50">
-        <v>963</v>
+      <c r="F50" t="str">
+        <f t="shared" si="0"/>
+        <v>Condo</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H50">
         <v>1</v>
       </c>
       <c r="J50" t="str">
-        <f t="shared" si="0"/>
-        <v>('202226090', '1650 Granville St #904, Halifax, NS B3J 0E1', 869000, 2, 2, 963, 'ardit@ucalgary.ca', 1),</v>
+        <f t="shared" si="1"/>
+        <v>('202226090', '1650 Granville St #904, Halifax, NS B3J 0E1', 869000, 2, 2, 'Condo', 'ardit@ucalgary.ca', 1),</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.35">
@@ -2965,18 +3014,19 @@
       <c r="E51">
         <v>2</v>
       </c>
-      <c r="F51">
-        <v>1688</v>
+      <c r="F51" t="str">
+        <f t="shared" si="0"/>
+        <v>House</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H51">
         <v>2</v>
       </c>
       <c r="J51" t="str">
-        <f t="shared" si="0"/>
-        <v>('202225003', '68 Hartlen Ave, Halifax, NS B3R 1R6', 379900, 3, 2, 1688, 'ardit@ucalgary.ca', 2),</v>
+        <f t="shared" si="1"/>
+        <v>('202225003', '68 Hartlen Ave, Halifax, NS B3R 1R6', 379900, 3, 2, 'House', 'ardit@ucalgary.ca', 2),</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.35">
@@ -2995,18 +3045,19 @@
       <c r="E52">
         <v>2</v>
       </c>
-      <c r="F52">
-        <v>1146</v>
+      <c r="F52" t="str">
+        <f t="shared" si="0"/>
+        <v>House</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H52">
         <v>3</v>
       </c>
       <c r="J52" t="str">
-        <f t="shared" si="0"/>
-        <v>('202223264', '1233 Purcells Cove Rd, Halifax, NS B3P 1B3', 499000, 3, 2, 1146, 'ardit@ucalgary.ca', 3),</v>
+        <f t="shared" si="1"/>
+        <v>('202223264', '1233 Purcells Cove Rd, Halifax, NS B3P 1B3', 499000, 3, 2, 'House', 'ardit@ucalgary.ca', 3),</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.35">
@@ -3025,18 +3076,19 @@
       <c r="E53">
         <v>3</v>
       </c>
-      <c r="F53">
-        <v>2720</v>
+      <c r="F53" t="str">
+        <f t="shared" si="0"/>
+        <v>House</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H53">
         <v>1</v>
       </c>
       <c r="J53" t="str">
-        <f t="shared" si="0"/>
-        <v>('202212337', '2947 Purcells Cove Rd, Halifax, NS B3P 2G2', 1995000, 3, 3, 2720, 'ardit@ucalgary.ca', 1),</v>
+        <f t="shared" si="1"/>
+        <v>('202212337', '2947 Purcells Cove Rd, Halifax, NS B3P 2G2', 1995000, 3, 3, 'House', 'ardit@ucalgary.ca', 1),</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.35">
@@ -3055,18 +3107,19 @@
       <c r="E54">
         <v>2</v>
       </c>
-      <c r="F54">
-        <v>1276</v>
+      <c r="F54" t="str">
+        <f t="shared" si="0"/>
+        <v>Condo</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H54">
         <v>2</v>
       </c>
       <c r="J54" t="str">
-        <f t="shared" si="0"/>
-        <v>('202224206', '13 McFatridge Rd, Halifax, NS B3N 2R2', 369900, 2, 2, 1276, 'ardit@ucalgary.ca', 2),</v>
+        <f t="shared" si="1"/>
+        <v>('202224206', '13 McFatridge Rd, Halifax, NS B3N 2R2', 369900, 2, 2, 'Condo', 'ardit@ucalgary.ca', 2),</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.35">
@@ -3085,18 +3138,19 @@
       <c r="E55">
         <v>2</v>
       </c>
-      <c r="F55">
-        <v>1981</v>
+      <c r="F55" t="str">
+        <f t="shared" si="0"/>
+        <v>House</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H55">
         <v>3</v>
       </c>
       <c r="J55" t="str">
-        <f t="shared" si="0"/>
-        <v>('202225587', '29 Gateway Rd, Halifax, NS B3M 1M6', 499900, 4, 2, 1981, 'ardit@ucalgary.ca', 3),</v>
+        <f t="shared" si="1"/>
+        <v>('202225587', '29 Gateway Rd, Halifax, NS B3M 1M6', 499900, 4, 2, 'House', 'ardit@ucalgary.ca', 3),</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.35">
@@ -3115,18 +3169,19 @@
       <c r="E56">
         <v>2</v>
       </c>
-      <c r="F56">
-        <v>940</v>
+      <c r="F56" t="str">
+        <f t="shared" si="0"/>
+        <v>Condo</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H56">
         <v>1</v>
       </c>
       <c r="J56" t="str">
-        <f t="shared" si="0"/>
-        <v>('R2738427', '1020 Harwood St #1504, Vancouver, BC V6E 4R1', 1199000, 2, 2, 940, 'ardit@ucalgary.ca', 1),</v>
+        <f t="shared" si="1"/>
+        <v>('R2738427', '1020 Harwood St #1504, Vancouver, BC V6E 4R1', 1199000, 2, 2, 'Condo', 'ardit@ucalgary.ca', 1),</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.35">
@@ -3145,18 +3200,19 @@
       <c r="E57">
         <v>1</v>
       </c>
-      <c r="F57">
-        <v>703</v>
+      <c r="F57" t="str">
+        <f t="shared" si="0"/>
+        <v>Condo</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H57">
         <v>2</v>
       </c>
       <c r="J57" t="str">
-        <f t="shared" si="0"/>
-        <v>('R2738459', '1718 Venables St #404, Vancouver, BC V5L 2H4', 689000, 1, 1, 703, 'ardit@ucalgary.ca', 2),</v>
+        <f t="shared" si="1"/>
+        <v>('R2738459', '1718 Venables St #404, Vancouver, BC V5L 2H4', 689000, 1, 1, 'Condo', 'ardit@ucalgary.ca', 2),</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.35">
@@ -3175,18 +3231,19 @@
       <c r="E58">
         <v>1</v>
       </c>
-      <c r="F58">
-        <v>538</v>
+      <c r="F58" t="str">
+        <f t="shared" si="0"/>
+        <v>Condo</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H58">
         <v>3</v>
       </c>
       <c r="J58" t="str">
-        <f t="shared" si="0"/>
-        <v>('R2738462', '1330 Burrard St #306, Vancouver, BC V6Z 2B8', 519000, 2, 1, 538, 'ardit@ucalgary.ca', 3),</v>
+        <f t="shared" si="1"/>
+        <v>('R2738462', '1330 Burrard St #306, Vancouver, BC V6Z 2B8', 519000, 2, 1, 'Condo', 'ardit@ucalgary.ca', 3),</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.35">
@@ -3205,18 +3262,19 @@
       <c r="E59">
         <v>4</v>
       </c>
-      <c r="F59">
-        <v>2445</v>
+      <c r="F59" t="str">
+        <f t="shared" si="0"/>
+        <v>House</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H59">
         <v>1</v>
       </c>
       <c r="J59" t="str">
-        <f t="shared" si="0"/>
-        <v>('R2738122', '4515 W 14th Ave, Vancouver, BC V6R 2Y5', 3088000, 5, 4, 2445, 'ardit@ucalgary.ca', 1),</v>
+        <f t="shared" si="1"/>
+        <v>('R2738122', '4515 W 14th Ave, Vancouver, BC V6R 2Y5', 3088000, 5, 4, 'House', 'ardit@ucalgary.ca', 1),</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.35">
@@ -3235,18 +3293,19 @@
       <c r="E60">
         <v>2</v>
       </c>
-      <c r="F60">
-        <v>2108</v>
+      <c r="F60" t="str">
+        <f t="shared" si="0"/>
+        <v>House</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H60">
         <v>2</v>
       </c>
       <c r="J60" t="str">
-        <f t="shared" si="0"/>
-        <v>('R2738271', '3678 E 25th Ave, Vancouver, BC V5R 1K5', 1788800, 4, 2, 2108, 'ardit@ucalgary.ca', 2),</v>
+        <f t="shared" si="1"/>
+        <v>('R2738271', '3678 E 25th Ave, Vancouver, BC V5R 1K5', 1788800, 4, 2, 'House', 'ardit@ucalgary.ca', 2),</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.35">
@@ -3265,18 +3324,19 @@
       <c r="E61">
         <v>9</v>
       </c>
-      <c r="F61">
-        <v>10880</v>
+      <c r="F61" t="str">
+        <f t="shared" si="0"/>
+        <v>House</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H61">
         <v>3</v>
       </c>
       <c r="J61" t="str">
-        <f t="shared" si="0"/>
-        <v>('R2738190', '3537 Osler St, Vancouver, BC V6H 2W4', 23800000, 5, 9, 10880, 'ardit@ucalgary.ca', 3),</v>
+        <f t="shared" si="1"/>
+        <v>('R2738190', '3537 Osler St, Vancouver, BC V6H 2W4', 23800000, 5, 9, 'House', 'ardit@ucalgary.ca', 3),</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.35">
@@ -3295,18 +3355,19 @@
       <c r="E62">
         <v>7</v>
       </c>
-      <c r="F62">
-        <v>6116</v>
+      <c r="F62" t="str">
+        <f t="shared" si="0"/>
+        <v>House</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H62">
         <v>1</v>
       </c>
       <c r="J62" t="str">
-        <f t="shared" si="0"/>
-        <v>('R2738436', '621 W 51st Ave, Vancouver, BC V6P 1B9', 4289000, 6, 7, 6116, 'ardit@ucalgary.ca', 1),</v>
+        <f t="shared" si="1"/>
+        <v>('R2738436', '621 W 51st Ave, Vancouver, BC V6P 1B9', 4289000, 6, 7, 'House', 'ardit@ucalgary.ca', 1),</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.35">
@@ -3325,18 +3386,19 @@
       <c r="E63">
         <v>9</v>
       </c>
-      <c r="F63">
-        <v>9949</v>
+      <c r="F63" t="str">
+        <f t="shared" si="0"/>
+        <v>House</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H63">
         <v>2</v>
       </c>
       <c r="J63" t="str">
-        <f t="shared" si="0"/>
-        <v>('R2697014', '1318 Minto Cres, Vancouver, BC V6H 2J5', 24800000, 5, 9, 9949, 'ardit@ucalgary.ca', 2),</v>
+        <f t="shared" si="1"/>
+        <v>('R2697014', '1318 Minto Cres, Vancouver, BC V6H 2J5', 24800000, 5, 9, 'House', 'ardit@ucalgary.ca', 2),</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.35">
@@ -3355,18 +3417,19 @@
       <c r="E64">
         <v>4</v>
       </c>
-      <c r="F64">
-        <v>2405</v>
+      <c r="F64" t="str">
+        <f t="shared" si="0"/>
+        <v>House</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H64">
         <v>3</v>
       </c>
       <c r="J64" t="str">
-        <f t="shared" si="0"/>
-        <v>('R2738458', '345 E 64th Ave, Vancouver, BC V5X 2M8', 1699000, 5, 4, 2405, 'ardit@ucalgary.ca', 3),</v>
+        <f t="shared" si="1"/>
+        <v>('R2738458', '345 E 64th Ave, Vancouver, BC V5X 2M8', 1699000, 5, 4, 'House', 'ardit@ucalgary.ca', 3),</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.35">
@@ -3385,18 +3448,19 @@
       <c r="E65">
         <v>2</v>
       </c>
-      <c r="F65">
-        <v>1380</v>
+      <c r="F65" t="str">
+        <f t="shared" si="0"/>
+        <v>House</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H65">
         <v>2</v>
       </c>
       <c r="J65" t="str">
-        <f t="shared" si="0"/>
-        <v>('R2738460', '137 Burrows Ave, Winnipeg, MB R2W 1Z3', 219900, 3, 2, 1380, 'ardit@ucalgary.ca', 2),</v>
+        <f t="shared" si="1"/>
+        <v>('R2738460', '137 Burrows Ave, Winnipeg, MB R2W 1Z3', 219900, 3, 2, 'House', 'ardit@ucalgary.ca', 2),</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.35">
@@ -3415,18 +3479,19 @@
       <c r="E66">
         <v>10</v>
       </c>
-      <c r="F66">
-        <v>12553</v>
+      <c r="F66" t="str">
+        <f t="shared" si="0"/>
+        <v>House</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H66">
         <v>3</v>
       </c>
       <c r="J66" t="str">
-        <f t="shared" si="0"/>
-        <v>('40181595', '1343 Blythe Rd, Mississauga, ON L5H 2C2', 24500000, 7, 10, 12553, 'ardit@ucalgary.ca', 3),</v>
+        <f t="shared" si="1"/>
+        <v>('40181595', '1343 Blythe Rd, Mississauga, ON L5H 2C2', 24500000, 7, 10, 'House', 'ardit@ucalgary.ca', 3),</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.35">
@@ -3445,18 +3510,19 @@
       <c r="E67">
         <v>2</v>
       </c>
-      <c r="F67">
-        <v>900</v>
+      <c r="F67" t="str">
+        <f t="shared" ref="F67:F130" si="2">IF(D67&lt;3, "Condo", "House")</f>
+        <v>House</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H67">
         <v>1</v>
       </c>
       <c r="J67" t="str">
-        <f t="shared" ref="J67:J130" si="1">_xlfn.CONCAT("('",A67, "'", ", ", "'", B67, "'", ", ", C67, ", ", D67, ", ", E67, ", ", F67, ", ", "'", G67, "'", ", ", H67, ")", ",")</f>
-        <v>('SK914132', '46 Peeling AVENUE, Saskatoon, SK S7M 4K4', 329900, 4, 2, 900, 'ardit@ucalgary.ca', 1),</v>
+        <f t="shared" ref="J67:J130" si="3">_xlfn.CONCAT("('",A67, "'", ", ", "'", B67, "'", ", ", C67, ", ", D67, ", ", E67, ", ", "'", F67, "'", ", ", "'", G67, "'", ", ", H67, ")", ",")</f>
+        <v>('SK914132', '46 Peeling AVENUE, Saskatoon, SK S7M 4K4', 329900, 4, 2, 'House', 'ardit@ucalgary.ca', 1),</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.35">
@@ -3475,18 +3541,19 @@
       <c r="E68">
         <v>3</v>
       </c>
-      <c r="F68">
-        <v>1144</v>
+      <c r="F68" t="str">
+        <f t="shared" si="2"/>
+        <v>House</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H68">
         <v>2</v>
       </c>
       <c r="J68" t="str">
-        <f t="shared" si="1"/>
-        <v>('SK914049', '831 F AVENUE N, Saskatoon, SK S7L 1W6', 419000, 5, 3, 1144, 'ardit@ucalgary.ca', 2),</v>
+        <f t="shared" si="3"/>
+        <v>('SK914049', '831 F AVENUE N, Saskatoon, SK S7L 1W6', 419000, 5, 3, 'House', 'ardit@ucalgary.ca', 2),</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.35">
@@ -3505,18 +3572,19 @@
       <c r="E69">
         <v>2</v>
       </c>
-      <c r="F69">
-        <v>835</v>
+      <c r="F69" t="str">
+        <f t="shared" si="2"/>
+        <v>House</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H69">
         <v>3</v>
       </c>
       <c r="J69" t="str">
-        <f t="shared" si="1"/>
-        <v>('SK914096', '739 L AVENUE S, Saskatoon, SK S7M 2H8', 229900, 3, 2, 835, 'ardit@ucalgary.ca', 3),</v>
+        <f t="shared" si="3"/>
+        <v>('SK914096', '739 L AVENUE S, Saskatoon, SK S7M 2H8', 229900, 3, 2, 'House', 'ardit@ucalgary.ca', 3),</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.35">
@@ -3535,18 +3603,19 @@
       <c r="E70">
         <v>1</v>
       </c>
-      <c r="F70">
-        <v>0</v>
+      <c r="F70" t="str">
+        <f t="shared" si="2"/>
+        <v>House</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H70">
         <v>3</v>
       </c>
       <c r="J70" t="str">
-        <f t="shared" si="1"/>
-        <v>('SK914089', '115 Ash STREET E, Saskatoon, SK', 259900, 3, 1, 0, 'ardit@ucalgary.ca', 3),</v>
+        <f t="shared" si="3"/>
+        <v>('SK914089', '115 Ash STREET E, Saskatoon, SK', 259900, 3, 1, 'House', 'ardit@ucalgary.ca', 3),</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.35">
@@ -3565,18 +3634,19 @@
       <c r="E71">
         <v>5</v>
       </c>
-      <c r="F71">
-        <v>0</v>
+      <c r="F71" t="str">
+        <f t="shared" si="2"/>
+        <v>House</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H71">
         <v>3</v>
       </c>
       <c r="J71" t="str">
-        <f t="shared" si="1"/>
-        <v>('SK914121', '1227 D AVENUE N, Saskatoon, SK', 249900, 8, 5, 0, 'ardit@ucalgary.ca', 3),</v>
+        <f t="shared" si="3"/>
+        <v>('SK914121', '1227 D AVENUE N, Saskatoon, SK', 249900, 8, 5, 'House', 'ardit@ucalgary.ca', 3),</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.35">
@@ -3595,18 +3665,19 @@
       <c r="E72">
         <v>3</v>
       </c>
-      <c r="F72">
-        <v>0</v>
+      <c r="F72" t="str">
+        <f t="shared" si="2"/>
+        <v>House</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H72">
         <v>1</v>
       </c>
       <c r="J72" t="str">
-        <f t="shared" si="1"/>
-        <v>('SK914104', '2415 Rosewood DRIVE, Saskatoon, SK', 598700, 3, 3, 0, 'ardit@ucalgary.ca', 1),</v>
+        <f t="shared" si="3"/>
+        <v>('SK914104', '2415 Rosewood DRIVE, Saskatoon, SK', 598700, 3, 3, 'House', 'ardit@ucalgary.ca', 1),</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.35">
@@ -3625,18 +3696,19 @@
       <c r="E73">
         <v>3</v>
       </c>
-      <c r="F73">
-        <v>0</v>
+      <c r="F73" t="str">
+        <f t="shared" si="2"/>
+        <v>Condo</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H73">
         <v>2</v>
       </c>
       <c r="J73" t="str">
-        <f t="shared" si="1"/>
-        <v>('SK914117', '1 927 Heritage VIEW, Saskatoon, SK', 509900, 2, 3, 0, 'ardit@ucalgary.ca', 2),</v>
+        <f t="shared" si="3"/>
+        <v>('SK914117', '1 927 Heritage VIEW, Saskatoon, SK', 509900, 2, 3, 'Condo', 'ardit@ucalgary.ca', 2),</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.35">
@@ -3655,18 +3727,19 @@
       <c r="E74">
         <v>3</v>
       </c>
-      <c r="F74">
-        <v>0</v>
+      <c r="F74" t="str">
+        <f t="shared" si="2"/>
+        <v>House</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H74">
         <v>1</v>
       </c>
       <c r="J74" t="str">
-        <f t="shared" si="1"/>
-        <v>('SK914106', '2427 Rosewood DRIVE, Saskatoon, SK', 632500, 4, 3, 0, 'ardit@ucalgary.ca', 1),</v>
+        <f t="shared" si="3"/>
+        <v>('SK914106', '2427 Rosewood DRIVE, Saskatoon, SK', 632500, 4, 3, 'House', 'ardit@ucalgary.ca', 1),</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.35">
@@ -3685,18 +3758,19 @@
       <c r="E75">
         <v>4</v>
       </c>
-      <c r="F75">
-        <v>0</v>
+      <c r="F75" t="str">
+        <f t="shared" si="2"/>
+        <v>House</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H75">
         <v>2</v>
       </c>
       <c r="J75" t="str">
-        <f t="shared" si="1"/>
-        <v>('SK914056', '3409 Ortona STREET, Saskatoon, SK', 1275000, 6, 4, 0, 'ardit@ucalgary.ca', 2),</v>
+        <f t="shared" si="3"/>
+        <v>('SK914056', '3409 Ortona STREET, Saskatoon, SK', 1275000, 6, 4, 'House', 'ardit@ucalgary.ca', 2),</v>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.35">
@@ -3715,18 +3789,19 @@
       <c r="E76">
         <v>3</v>
       </c>
-      <c r="F76">
-        <v>0</v>
+      <c r="F76" t="str">
+        <f t="shared" si="2"/>
+        <v>House</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H76">
         <v>1</v>
       </c>
       <c r="J76" t="str">
-        <f t="shared" si="1"/>
-        <v>('SK913998', '302 Poth CRESCENT, Saskatoon, SK', 319900, 3, 3, 0, 'ardit@ucalgary.ca', 1),</v>
+        <f t="shared" si="3"/>
+        <v>('SK913998', '302 Poth CRESCENT, Saskatoon, SK', 319900, 3, 3, 'House', 'ardit@ucalgary.ca', 1),</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.35">
@@ -3745,18 +3820,19 @@
       <c r="E77">
         <v>3</v>
       </c>
-      <c r="F77">
-        <v>0</v>
+      <c r="F77" t="str">
+        <f t="shared" si="2"/>
+        <v>House</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H77">
         <v>2</v>
       </c>
       <c r="J77" t="str">
-        <f t="shared" si="1"/>
-        <v>('SK914012', '652 University DRIVE, Saskatoon, SK', 599900, 5, 3, 0, 'ardit@ucalgary.ca', 2),</v>
+        <f t="shared" si="3"/>
+        <v>('SK914012', '652 University DRIVE, Saskatoon, SK', 599900, 5, 3, 'House', 'ardit@ucalgary.ca', 2),</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.35">
@@ -3775,18 +3851,19 @@
       <c r="E78">
         <v>1</v>
       </c>
-      <c r="F78">
-        <v>0</v>
+      <c r="F78" t="str">
+        <f t="shared" si="2"/>
+        <v>Condo</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H78">
         <v>3</v>
       </c>
       <c r="J78" t="str">
-        <f t="shared" si="1"/>
-        <v>('SK914042', '108 1435 Embassy DRIVE, Saskatoon, SK', 119900, 2, 1, 0, 'ardit@ucalgary.ca', 3),</v>
+        <f t="shared" si="3"/>
+        <v>('SK914042', '108 1435 Embassy DRIVE, Saskatoon, SK', 119900, 2, 1, 'Condo', 'ardit@ucalgary.ca', 3),</v>
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.35">
@@ -3805,18 +3882,19 @@
       <c r="E79">
         <v>1</v>
       </c>
-      <c r="F79">
-        <v>0</v>
+      <c r="F79" t="str">
+        <f t="shared" si="2"/>
+        <v>Condo</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H79">
         <v>1</v>
       </c>
       <c r="J79" t="str">
-        <f t="shared" si="1"/>
-        <v>('SK914035', '506 537 4th AVENUE N, Saskatoon, SK', 179900, 2, 1, 0, 'ardit@ucalgary.ca', 1),</v>
+        <f t="shared" si="3"/>
+        <v>('SK914035', '506 537 4th AVENUE N, Saskatoon, SK', 179900, 2, 1, 'Condo', 'ardit@ucalgary.ca', 1),</v>
       </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.35">
@@ -3835,18 +3913,19 @@
       <c r="E80">
         <v>2</v>
       </c>
-      <c r="F80">
-        <v>0</v>
+      <c r="F80" t="str">
+        <f t="shared" si="2"/>
+        <v>Condo</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H80">
         <v>2</v>
       </c>
       <c r="J80" t="str">
-        <f t="shared" si="1"/>
-        <v>('SK914010', 'B4 255 Kingsmere BOULEVARD, Saskatoon, SK', 129900, 2, 2, 0, 'ardit@ucalgary.ca', 2),</v>
+        <f t="shared" si="3"/>
+        <v>('SK914010', 'B4 255 Kingsmere BOULEVARD, Saskatoon, SK', 129900, 2, 2, 'Condo', 'ardit@ucalgary.ca', 2),</v>
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.35">
@@ -3865,18 +3944,19 @@
       <c r="E81">
         <v>3</v>
       </c>
-      <c r="F81">
-        <v>0</v>
+      <c r="F81" t="str">
+        <f t="shared" si="2"/>
+        <v>House</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H81">
         <v>3</v>
       </c>
       <c r="J81" t="str">
-        <f t="shared" si="1"/>
-        <v>('SK914052', '210 Aniskotaw MANOR, Saskatoon, SK', 499900, 3, 3, 0, 'ardit@ucalgary.ca', 3),</v>
+        <f t="shared" si="3"/>
+        <v>('SK914052', '210 Aniskotaw MANOR, Saskatoon, SK', 499900, 3, 3, 'House', 'ardit@ucalgary.ca', 3),</v>
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.35">
@@ -3895,18 +3975,19 @@
       <c r="E82">
         <v>3</v>
       </c>
-      <c r="F82">
-        <v>0</v>
+      <c r="F82" t="str">
+        <f t="shared" si="2"/>
+        <v>House</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H82">
         <v>2</v>
       </c>
       <c r="J82" t="str">
-        <f t="shared" si="1"/>
-        <v>('E4319228', '14425 110A AV NW, Edmonton, AB', 392500, 4, 3, 0, 'ardit@ucalgary.ca', 2),</v>
+        <f t="shared" si="3"/>
+        <v>('E4319228', '14425 110A AV NW, Edmonton, AB', 392500, 4, 3, 'House', 'ardit@ucalgary.ca', 2),</v>
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.35">
@@ -3925,18 +4006,19 @@
       <c r="E83">
         <v>3</v>
       </c>
-      <c r="F83">
-        <v>0</v>
+      <c r="F83" t="str">
+        <f t="shared" si="2"/>
+        <v>House</v>
       </c>
       <c r="G83" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H83">
         <v>3</v>
       </c>
       <c r="J83" t="str">
-        <f t="shared" si="1"/>
-        <v>('E4318803', '9124 141 ST NW NW, Edmonton, AB', 1190000, 4, 3, 0, 'ardit@ucalgary.ca', 3),</v>
+        <f t="shared" si="3"/>
+        <v>('E4318803', '9124 141 ST NW NW, Edmonton, AB', 1190000, 4, 3, 'House', 'ardit@ucalgary.ca', 3),</v>
       </c>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.35">
@@ -3955,18 +4037,19 @@
       <c r="E84">
         <v>2</v>
       </c>
-      <c r="F84">
-        <v>0</v>
+      <c r="F84" t="str">
+        <f t="shared" si="2"/>
+        <v>House</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H84">
         <v>1</v>
       </c>
       <c r="J84" t="str">
-        <f t="shared" si="1"/>
-        <v>('E4318797', '#7 15710 BEAUMARIS RD NW, Edmonton, AB', 189900, 3, 2, 0, 'ardit@ucalgary.ca', 1),</v>
+        <f t="shared" si="3"/>
+        <v>('E4318797', '#7 15710 BEAUMARIS RD NW, Edmonton, AB', 189900, 3, 2, 'House', 'ardit@ucalgary.ca', 1),</v>
       </c>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.35">
@@ -3985,18 +4068,19 @@
       <c r="E85">
         <v>2</v>
       </c>
-      <c r="F85">
-        <v>0</v>
+      <c r="F85" t="str">
+        <f t="shared" si="2"/>
+        <v>House</v>
       </c>
       <c r="G85" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H85">
         <v>2</v>
       </c>
       <c r="J85" t="str">
-        <f t="shared" si="1"/>
-        <v>('E4318817', '6843 111 ST NW, Edmonton, AB', 380000, 4, 2, 0, 'ardit@ucalgary.ca', 2),</v>
+        <f t="shared" si="3"/>
+        <v>('E4318817', '6843 111 ST NW, Edmonton, AB', 380000, 4, 2, 'House', 'ardit@ucalgary.ca', 2),</v>
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.35">
@@ -4015,18 +4099,19 @@
       <c r="E86">
         <v>2</v>
       </c>
-      <c r="F86">
-        <v>0</v>
+      <c r="F86" t="str">
+        <f t="shared" si="2"/>
+        <v>Condo</v>
       </c>
       <c r="G86" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H86">
         <v>3</v>
       </c>
       <c r="J86" t="str">
-        <f t="shared" si="1"/>
-        <v>('E4318811', '#602 12303 JASPER AV NW, Edmonton, AB', 325000, 2, 2, 0, 'ardit@ucalgary.ca', 3),</v>
+        <f t="shared" si="3"/>
+        <v>('E4318811', '#602 12303 JASPER AV NW, Edmonton, AB', 325000, 2, 2, 'Condo', 'ardit@ucalgary.ca', 3),</v>
       </c>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.35">
@@ -4045,18 +4130,19 @@
       <c r="E87">
         <v>2</v>
       </c>
-      <c r="F87">
-        <v>0</v>
+      <c r="F87" t="str">
+        <f t="shared" si="2"/>
+        <v>House</v>
       </c>
       <c r="G87" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H87">
         <v>1</v>
       </c>
       <c r="J87" t="str">
-        <f t="shared" si="1"/>
-        <v>('E4318805', '11710 122 ST NW, Edmonton, AB', 389900, 3, 2, 0, 'ardit@ucalgary.ca', 1),</v>
+        <f t="shared" si="3"/>
+        <v>('E4318805', '11710 122 ST NW, Edmonton, AB', 389900, 3, 2, 'House', 'ardit@ucalgary.ca', 1),</v>
       </c>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.35">
@@ -4075,18 +4161,19 @@
       <c r="E88">
         <v>1</v>
       </c>
-      <c r="F88">
-        <v>0</v>
+      <c r="F88" t="str">
+        <f t="shared" si="2"/>
+        <v>Condo</v>
       </c>
       <c r="G88" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H88">
         <v>2</v>
       </c>
       <c r="J88" t="str">
-        <f t="shared" si="1"/>
-        <v>('E4318453', '#1502 10303 105 ST NW, Edmonton, AB', 215000, 2, 1, 0, 'ardit@ucalgary.ca', 2),</v>
+        <f t="shared" si="3"/>
+        <v>('E4318453', '#1502 10303 105 ST NW, Edmonton, AB', 215000, 2, 1, 'Condo', 'ardit@ucalgary.ca', 2),</v>
       </c>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.35">
@@ -4105,18 +4192,19 @@
       <c r="E89">
         <v>6</v>
       </c>
-      <c r="F89">
-        <v>0</v>
+      <c r="F89" t="str">
+        <f t="shared" si="2"/>
+        <v>House</v>
       </c>
       <c r="G89" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H89">
         <v>3</v>
       </c>
       <c r="J89" t="str">
-        <f t="shared" si="1"/>
-        <v>('E4318462', '16 West Point WD NW, Edmonton, AB', 1389900, 4, 6, 0, 'ardit@ucalgary.ca', 3),</v>
+        <f t="shared" si="3"/>
+        <v>('E4318462', '16 West Point WD NW, Edmonton, AB', 1389900, 4, 6, 'House', 'ardit@ucalgary.ca', 3),</v>
       </c>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.35">
@@ -4135,18 +4223,19 @@
       <c r="E90">
         <v>4</v>
       </c>
-      <c r="F90">
-        <v>0</v>
+      <c r="F90" t="str">
+        <f t="shared" si="2"/>
+        <v>House</v>
       </c>
       <c r="G90" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H90">
         <v>1</v>
       </c>
       <c r="J90" t="str">
-        <f t="shared" si="1"/>
-        <v>('E4318292', '9220 75 ST NW, Edmonton, AB', 450000, 5, 4, 0, 'ardit@ucalgary.ca', 1),</v>
+        <f t="shared" si="3"/>
+        <v>('E4318292', '9220 75 ST NW, Edmonton, AB', 450000, 5, 4, 'House', 'ardit@ucalgary.ca', 1),</v>
       </c>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.35">
@@ -4165,18 +4254,19 @@
       <c r="E91">
         <v>1</v>
       </c>
-      <c r="F91">
-        <v>0</v>
+      <c r="F91" t="str">
+        <f t="shared" si="2"/>
+        <v>Condo</v>
       </c>
       <c r="G91" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H91">
         <v>2</v>
       </c>
       <c r="J91" t="str">
-        <f t="shared" si="1"/>
-        <v>('E4318289', '#120 10407 122 ST NW, Edmonton, AB', 234800, 2, 1, 0, 'ardit@ucalgary.ca', 2),</v>
+        <f t="shared" si="3"/>
+        <v>('E4318289', '#120 10407 122 ST NW, Edmonton, AB', 234800, 2, 1, 'Condo', 'ardit@ucalgary.ca', 2),</v>
       </c>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.35">
@@ -4195,18 +4285,19 @@
       <c r="E92">
         <v>2</v>
       </c>
-      <c r="F92">
-        <v>0</v>
+      <c r="F92" t="str">
+        <f t="shared" si="2"/>
+        <v>Condo</v>
       </c>
       <c r="G92" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H92">
         <v>3</v>
       </c>
       <c r="J92" t="str">
-        <f t="shared" si="1"/>
-        <v>('E4318264', '11134 101 ST NW, Edmonton, AB', 309900, 2, 2, 0, 'ardit@ucalgary.ca', 3),</v>
+        <f t="shared" si="3"/>
+        <v>('E4318264', '11134 101 ST NW, Edmonton, AB', 309900, 2, 2, 'Condo', 'ardit@ucalgary.ca', 3),</v>
       </c>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.35">
@@ -4225,18 +4316,19 @@
       <c r="E93">
         <v>1</v>
       </c>
-      <c r="F93">
-        <v>0</v>
+      <c r="F93" t="str">
+        <f t="shared" si="2"/>
+        <v>Condo</v>
       </c>
       <c r="G93" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H93">
         <v>1</v>
       </c>
       <c r="J93" t="str">
-        <f t="shared" si="1"/>
-        <v>('E4318270', '12824 130 ST NW, Edmonton, AB', 286900, 2, 1, 0, 'ardit@ucalgary.ca', 1),</v>
+        <f t="shared" si="3"/>
+        <v>('E4318270', '12824 130 ST NW, Edmonton, AB', 286900, 2, 1, 'Condo', 'ardit@ucalgary.ca', 1),</v>
       </c>
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.35">
@@ -4255,18 +4347,19 @@
       <c r="E94">
         <v>4</v>
       </c>
-      <c r="F94">
-        <v>0</v>
+      <c r="F94" t="str">
+        <f t="shared" si="2"/>
+        <v>House</v>
       </c>
       <c r="G94" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H94">
         <v>2</v>
       </c>
       <c r="J94" t="str">
-        <f t="shared" si="1"/>
-        <v>('E4318272', '6512 111 AV NW, Edmonton, AB', 835000, 5, 4, 0, 'ardit@ucalgary.ca', 2),</v>
+        <f t="shared" si="3"/>
+        <v>('E4318272', '6512 111 AV NW, Edmonton, AB', 835000, 5, 4, 'House', 'ardit@ucalgary.ca', 2),</v>
       </c>
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.35">
@@ -4285,18 +4378,19 @@
       <c r="E95">
         <v>2</v>
       </c>
-      <c r="F95">
-        <v>0</v>
+      <c r="F95" t="str">
+        <f t="shared" si="2"/>
+        <v>Condo</v>
       </c>
       <c r="G95" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H95">
         <v>3</v>
       </c>
       <c r="J95" t="str">
-        <f t="shared" si="1"/>
-        <v>('E4318286', '#809 10142 111 ST NW, Edmonton, AB', 400000, 2, 2, 0, 'feras@ucalgary.ca', 3),</v>
+        <f t="shared" si="3"/>
+        <v>('E4318286', '#809 10142 111 ST NW, Edmonton, AB', 400000, 2, 2, 'Condo', 'feras@ucalgary.ca', 3),</v>
       </c>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.35">
@@ -4315,18 +4409,19 @@
       <c r="E96">
         <v>1</v>
       </c>
-      <c r="F96">
-        <v>0</v>
+      <c r="F96" t="str">
+        <f t="shared" si="2"/>
+        <v>Condo</v>
       </c>
       <c r="G96" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H96">
         <v>1</v>
       </c>
       <c r="J96" t="str">
-        <f t="shared" si="1"/>
-        <v>('A2004671', '12905 66 Street NW, Edmonton, AB', 250000, 2, 1, 0, 'feras@ucalgary.ca', 1),</v>
+        <f t="shared" si="3"/>
+        <v>('A2004671', '12905 66 Street NW, Edmonton, AB', 250000, 2, 1, 'Condo', 'feras@ucalgary.ca', 1),</v>
       </c>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.35">
@@ -4345,18 +4440,19 @@
       <c r="E97">
         <v>5</v>
       </c>
-      <c r="F97">
-        <v>0</v>
+      <c r="F97" t="str">
+        <f t="shared" si="2"/>
+        <v>House</v>
       </c>
       <c r="G97" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H97">
         <v>2</v>
       </c>
       <c r="J97" t="str">
-        <f t="shared" si="1"/>
-        <v>('E4313860', '9535 147 AV NW, Edmonton, AB', 295000, 4, 5, 0, 'feras@ucalgary.ca', 2),</v>
+        <f t="shared" si="3"/>
+        <v>('E4313860', '9535 147 AV NW, Edmonton, AB', 295000, 4, 5, 'House', 'feras@ucalgary.ca', 2),</v>
       </c>
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.35">
@@ -4375,18 +4471,19 @@
       <c r="E98">
         <v>2</v>
       </c>
-      <c r="F98">
-        <v>0</v>
+      <c r="F98" t="str">
+        <f t="shared" si="2"/>
+        <v>Condo</v>
       </c>
       <c r="G98" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H98">
         <v>3</v>
       </c>
       <c r="J98" t="str">
-        <f t="shared" si="1"/>
-        <v>('E4313357', '#105 11716 100 AV NW, Edmonton, AB', 320000, 2, 2, 0, 'feras@ucalgary.ca', 3),</v>
+        <f t="shared" si="3"/>
+        <v>('E4313357', '#105 11716 100 AV NW, Edmonton, AB', 320000, 2, 2, 'Condo', 'feras@ucalgary.ca', 3),</v>
       </c>
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.35">
@@ -4405,18 +4502,19 @@
       <c r="E99">
         <v>2</v>
       </c>
-      <c r="F99">
-        <v>0</v>
+      <c r="F99" t="str">
+        <f t="shared" si="2"/>
+        <v>Condo</v>
       </c>
       <c r="G99" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H99">
         <v>1</v>
       </c>
       <c r="J99" t="str">
-        <f t="shared" si="1"/>
-        <v>('A2009409', '253 22 Avenue NW, Calgary, AB', 629999, 2, 2, 0, 'feras@ucalgary.ca', 1),</v>
+        <f t="shared" si="3"/>
+        <v>('A2009409', '253 22 Avenue NW, Calgary, AB', 629999, 2, 2, 'Condo', 'feras@ucalgary.ca', 1),</v>
       </c>
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.35">
@@ -4435,18 +4533,19 @@
       <c r="E100">
         <v>4</v>
       </c>
-      <c r="F100">
-        <v>0</v>
+      <c r="F100" t="str">
+        <f t="shared" si="2"/>
+        <v>House</v>
       </c>
       <c r="G100" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H100">
         <v>2</v>
       </c>
       <c r="J100" t="str">
-        <f t="shared" si="1"/>
-        <v>('A2008802', '159 New Brighton Close SE, Calgary, AB', 689900, 5, 4, 0, 'feras@ucalgary.ca', 2),</v>
+        <f t="shared" si="3"/>
+        <v>('A2008802', '159 New Brighton Close SE, Calgary, AB', 689900, 5, 4, 'House', 'feras@ucalgary.ca', 2),</v>
       </c>
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.35">
@@ -4465,18 +4564,19 @@
       <c r="E101">
         <v>2</v>
       </c>
-      <c r="F101">
-        <v>0</v>
+      <c r="F101" t="str">
+        <f t="shared" si="2"/>
+        <v>House</v>
       </c>
       <c r="G101" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H101">
         <v>3</v>
       </c>
       <c r="J101" t="str">
-        <f t="shared" si="1"/>
-        <v>('A2003495', '1029 Fonda Court SE, Calgary, AB', 299900, 4, 2, 0, 'feras@ucalgary.ca', 3),</v>
+        <f t="shared" si="3"/>
+        <v>('A2003495', '1029 Fonda Court SE, Calgary, AB', 299900, 4, 2, 'House', 'feras@ucalgary.ca', 3),</v>
       </c>
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.35">
@@ -4495,18 +4595,19 @@
       <c r="E102">
         <v>3</v>
       </c>
-      <c r="F102">
-        <v>0</v>
+      <c r="F102" t="str">
+        <f t="shared" si="2"/>
+        <v>House</v>
       </c>
       <c r="G102" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H102">
         <v>1</v>
       </c>
       <c r="J102" t="str">
-        <f t="shared" si="1"/>
-        <v>('A2005616', '1716 42 Street NE, Calgary, AB', 519900, 4, 3, 0, 'feras@ucalgary.ca', 1),</v>
+        <f t="shared" si="3"/>
+        <v>('A2005616', '1716 42 Street NE, Calgary, AB', 519900, 4, 3, 'House', 'feras@ucalgary.ca', 1),</v>
       </c>
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.35">
@@ -4525,18 +4626,19 @@
       <c r="E103">
         <v>2</v>
       </c>
-      <c r="F103">
-        <v>0</v>
+      <c r="F103" t="str">
+        <f t="shared" si="2"/>
+        <v>House</v>
       </c>
       <c r="G103" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H103">
         <v>2</v>
       </c>
       <c r="J103" t="str">
-        <f t="shared" si="1"/>
-        <v>('A2011129', '111 Deerpath Court SE, Calgary, AB', 399000, 3, 2, 0, 'feras@ucalgary.ca', 2),</v>
+        <f t="shared" si="3"/>
+        <v>('A2011129', '111 Deerpath Court SE, Calgary, AB', 399000, 3, 2, 'House', 'feras@ucalgary.ca', 2),</v>
       </c>
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.35">
@@ -4555,18 +4657,19 @@
       <c r="E104">
         <v>4</v>
       </c>
-      <c r="F104">
-        <v>0</v>
+      <c r="F104" t="str">
+        <f t="shared" si="2"/>
+        <v>House</v>
       </c>
       <c r="G104" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H104">
         <v>3</v>
       </c>
       <c r="J104" t="str">
-        <f t="shared" si="1"/>
-        <v>('A2012027', '1 1720 kensington Road NW, Calgary, AB', 575000, 3, 4, 0, 'feras@ucalgary.ca', 3),</v>
+        <f t="shared" si="3"/>
+        <v>('A2012027', '1 1720 kensington Road NW, Calgary, AB', 575000, 3, 4, 'House', 'feras@ucalgary.ca', 3),</v>
       </c>
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.35">
@@ -4585,18 +4688,19 @@
       <c r="E105">
         <v>2</v>
       </c>
-      <c r="F105">
-        <v>0</v>
+      <c r="F105" t="str">
+        <f t="shared" si="2"/>
+        <v>House</v>
       </c>
       <c r="G105" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H105">
         <v>1</v>
       </c>
       <c r="J105" t="str">
-        <f t="shared" si="1"/>
-        <v>('A2011096', '180 Gordon Drive SW, Calgary, AB', 499900, 3, 2, 0, 'feras@ucalgary.ca', 1),</v>
+        <f t="shared" si="3"/>
+        <v>('A2011096', '180 Gordon Drive SW, Calgary, AB', 499900, 3, 2, 'House', 'feras@ucalgary.ca', 1),</v>
       </c>
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.35">
@@ -4615,18 +4719,19 @@
       <c r="E106">
         <v>1</v>
       </c>
-      <c r="F106">
-        <v>0</v>
+      <c r="F106" t="str">
+        <f t="shared" si="2"/>
+        <v>Condo</v>
       </c>
       <c r="G106" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H106">
         <v>2</v>
       </c>
       <c r="J106" t="str">
-        <f t="shared" si="1"/>
-        <v>('A2011719', '2 930 Royal Avenue SW, Calgary, AB', 199900, 2, 1, 0, 'feras@ucalgary.ca', 2),</v>
+        <f t="shared" si="3"/>
+        <v>('A2011719', '2 930 Royal Avenue SW, Calgary, AB', 199900, 2, 1, 'Condo', 'feras@ucalgary.ca', 2),</v>
       </c>
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.35">
@@ -4645,18 +4750,19 @@
       <c r="E107">
         <v>1</v>
       </c>
-      <c r="F107">
-        <v>0</v>
+      <c r="F107" t="str">
+        <f t="shared" si="2"/>
+        <v>Condo</v>
       </c>
       <c r="G107" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H107">
         <v>3</v>
       </c>
       <c r="J107" t="str">
-        <f t="shared" si="1"/>
-        <v>('A2011914', '1413 151 Country Village Road NE, Calgary, AB', 340000, 1, 1, 0, 'feras@ucalgary.ca', 3),</v>
+        <f t="shared" si="3"/>
+        <v>('A2011914', '1413 151 Country Village Road NE, Calgary, AB', 340000, 1, 1, 'Condo', 'feras@ucalgary.ca', 3),</v>
       </c>
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.35">
@@ -4675,18 +4781,19 @@
       <c r="E108">
         <v>2</v>
       </c>
-      <c r="F108">
-        <v>0</v>
+      <c r="F108" t="str">
+        <f t="shared" si="2"/>
+        <v>House</v>
       </c>
       <c r="G108" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H108">
         <v>1</v>
       </c>
       <c r="J108" t="str">
-        <f t="shared" si="1"/>
-        <v>('A2012019', '27 Hunterhorn Crescent NE, Calgary, AB', 349900, 3, 2, 0, 'feras@ucalgary.ca', 1),</v>
+        <f t="shared" si="3"/>
+        <v>('A2012019', '27 Hunterhorn Crescent NE, Calgary, AB', 349900, 3, 2, 'House', 'feras@ucalgary.ca', 1),</v>
       </c>
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.35">
@@ -4705,18 +4812,19 @@
       <c r="E109">
         <v>3</v>
       </c>
-      <c r="F109">
-        <v>0</v>
+      <c r="F109" t="str">
+        <f t="shared" si="2"/>
+        <v>House</v>
       </c>
       <c r="G109" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H109">
         <v>2</v>
       </c>
       <c r="J109" t="str">
-        <f t="shared" si="1"/>
-        <v>('A2007664', '325 Mckenzie Towne Gate SE, Calgary, AB', 374900, 3, 3, 0, 'feras@ucalgary.ca', 2),</v>
+        <f t="shared" si="3"/>
+        <v>('A2007664', '325 Mckenzie Towne Gate SE, Calgary, AB', 374900, 3, 3, 'House', 'feras@ucalgary.ca', 2),</v>
       </c>
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.35">
@@ -4735,18 +4843,19 @@
       <c r="E110">
         <v>2</v>
       </c>
-      <c r="F110">
-        <v>0</v>
+      <c r="F110" t="str">
+        <f t="shared" si="2"/>
+        <v>House</v>
       </c>
       <c r="G110" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H110">
         <v>3</v>
       </c>
       <c r="J110" t="str">
-        <f t="shared" si="1"/>
-        <v>('A2009419', '8 Taraglen Road NE, Calgary, AB', 439900, 3, 2, 0, 'feras@ucalgary.ca', 3),</v>
+        <f t="shared" si="3"/>
+        <v>('A2009419', '8 Taraglen Road NE, Calgary, AB', 439900, 3, 2, 'House', 'feras@ucalgary.ca', 3),</v>
       </c>
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.35">
@@ -4765,18 +4874,19 @@
       <c r="E111">
         <v>1</v>
       </c>
-      <c r="F111">
-        <v>0</v>
+      <c r="F111" t="str">
+        <f t="shared" si="2"/>
+        <v>Condo</v>
       </c>
       <c r="G111" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H111">
         <v>1</v>
       </c>
       <c r="J111" t="str">
-        <f t="shared" si="1"/>
-        <v>('A1258735', '4308 13045 6 Street SW, Calgary, AB', 174900, 2, 1, 0, 'feras@ucalgary.ca', 1),</v>
+        <f t="shared" si="3"/>
+        <v>('A1258735', '4308 13045 6 Street SW, Calgary, AB', 174900, 2, 1, 'Condo', 'feras@ucalgary.ca', 1),</v>
       </c>
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.35">
@@ -4795,18 +4905,19 @@
       <c r="E112">
         <v>4</v>
       </c>
-      <c r="F112">
-        <v>0</v>
+      <c r="F112" t="str">
+        <f t="shared" si="2"/>
+        <v>House</v>
       </c>
       <c r="G112" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H112">
         <v>2</v>
       </c>
       <c r="J112" t="str">
-        <f t="shared" si="1"/>
-        <v>('A2010155', '106 Tuscany Meadows Heights NW, Calgary, AB', 924888, 4, 4, 0, 'feras@ucalgary.ca', 2),</v>
+        <f t="shared" si="3"/>
+        <v>('A2010155', '106 Tuscany Meadows Heights NW, Calgary, AB', 924888, 4, 4, 'House', 'feras@ucalgary.ca', 2),</v>
       </c>
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.35">
@@ -4825,18 +4936,19 @@
       <c r="E113">
         <v>1</v>
       </c>
-      <c r="F113">
-        <v>0</v>
+      <c r="F113" t="str">
+        <f t="shared" si="2"/>
+        <v>Condo</v>
       </c>
       <c r="G113" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H113">
         <v>3</v>
       </c>
       <c r="J113" t="str">
-        <f t="shared" si="1"/>
-        <v>('A2004459', '305 525 13 Avenue SW, Calgary, AB', 159900, 1, 1, 0, 'feras@ucalgary.ca', 3),</v>
+        <f t="shared" si="3"/>
+        <v>('A2004459', '305 525 13 Avenue SW, Calgary, AB', 159900, 1, 1, 'Condo', 'feras@ucalgary.ca', 3),</v>
       </c>
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.35">
@@ -4855,18 +4967,19 @@
       <c r="E114">
         <v>2</v>
       </c>
-      <c r="F114">
-        <v>0</v>
+      <c r="F114" t="str">
+        <f t="shared" si="2"/>
+        <v>Condo</v>
       </c>
       <c r="G114" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H114">
         <v>1</v>
       </c>
       <c r="J114" t="str">
-        <f t="shared" si="1"/>
-        <v>('A2008620', '306 1315 12 Avenue SW, Calgary, AB', 294900, 2, 2, 0, 'feras@ucalgary.ca', 1),</v>
+        <f t="shared" si="3"/>
+        <v>('A2008620', '306 1315 12 Avenue SW, Calgary, AB', 294900, 2, 2, 'Condo', 'feras@ucalgary.ca', 1),</v>
       </c>
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.35">
@@ -4885,18 +4998,19 @@
       <c r="E115">
         <v>3</v>
       </c>
-      <c r="F115">
-        <v>0</v>
+      <c r="F115" t="str">
+        <f t="shared" si="2"/>
+        <v>House</v>
       </c>
       <c r="G115" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H115">
         <v>2</v>
       </c>
       <c r="J115" t="str">
-        <f t="shared" si="1"/>
-        <v>('A2003939', '40 Strathcona Road SW, Calgary, AB', 699900, 3, 3, 0, 'feras@ucalgary.ca', 2),</v>
+        <f t="shared" si="3"/>
+        <v>('A2003939', '40 Strathcona Road SW, Calgary, AB', 699900, 3, 3, 'House', 'feras@ucalgary.ca', 2),</v>
       </c>
     </row>
     <row r="116" spans="1:10" x14ac:dyDescent="0.35">
@@ -4915,18 +5029,19 @@
       <c r="E116">
         <v>3</v>
       </c>
-      <c r="F116">
-        <v>0</v>
+      <c r="F116" t="str">
+        <f t="shared" si="2"/>
+        <v>House</v>
       </c>
       <c r="G116" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H116">
         <v>3</v>
       </c>
       <c r="J116" t="str">
-        <f t="shared" si="1"/>
-        <v>('A2009522', '34 New Brighton Circle SE, Calgary, AB', 559900, 3, 3, 0, 'feras@ucalgary.ca', 3),</v>
+        <f t="shared" si="3"/>
+        <v>('A2009522', '34 New Brighton Circle SE, Calgary, AB', 559900, 3, 3, 'House', 'feras@ucalgary.ca', 3),</v>
       </c>
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.35">
@@ -4945,18 +5060,19 @@
       <c r="E117">
         <v>1</v>
       </c>
-      <c r="F117">
-        <v>0</v>
+      <c r="F117" t="str">
+        <f t="shared" si="2"/>
+        <v>Condo</v>
       </c>
       <c r="G117" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H117">
         <v>1</v>
       </c>
       <c r="J117" t="str">
-        <f t="shared" si="1"/>
-        <v>('A2004597', '1115 2395 Eversyde Avenue SW, Calgary, AB', 224900, 2, 1, 0, 'feras@ucalgary.ca', 1),</v>
+        <f t="shared" si="3"/>
+        <v>('A2004597', '1115 2395 Eversyde Avenue SW, Calgary, AB', 224900, 2, 1, 'Condo', 'feras@ucalgary.ca', 1),</v>
       </c>
     </row>
     <row r="118" spans="1:10" x14ac:dyDescent="0.35">
@@ -4975,18 +5091,19 @@
       <c r="E118">
         <v>2</v>
       </c>
-      <c r="F118">
-        <v>0</v>
+      <c r="F118" t="str">
+        <f t="shared" si="2"/>
+        <v>Condo</v>
       </c>
       <c r="G118" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H118">
         <v>2</v>
       </c>
       <c r="J118" t="str">
-        <f t="shared" si="1"/>
-        <v>('A1255646', '3101 73 Erin Woods Court SE, Calgary, AB', 209900, 2, 2, 0, 'feras@ucalgary.ca', 2),</v>
+        <f t="shared" si="3"/>
+        <v>('A1255646', '3101 73 Erin Woods Court SE, Calgary, AB', 209900, 2, 2, 'Condo', 'feras@ucalgary.ca', 2),</v>
       </c>
     </row>
     <row r="119" spans="1:10" x14ac:dyDescent="0.35">
@@ -5005,18 +5122,19 @@
       <c r="E119">
         <v>1</v>
       </c>
-      <c r="F119">
-        <v>0</v>
+      <c r="F119" t="str">
+        <f t="shared" si="2"/>
+        <v>Condo</v>
       </c>
       <c r="G119" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H119">
         <v>3</v>
       </c>
       <c r="J119" t="str">
-        <f t="shared" si="1"/>
-        <v>('C5827918', '#423 1005 KING ST W, Toronto, ON', 629000, 1, 1, 0, 'feras@ucalgary.ca', 3),</v>
+        <f t="shared" si="3"/>
+        <v>('C5827918', '#423 1005 KING ST W, Toronto, ON', 629000, 1, 1, 'Condo', 'feras@ucalgary.ca', 3),</v>
       </c>
     </row>
     <row r="120" spans="1:10" x14ac:dyDescent="0.35">
@@ -5035,18 +5153,19 @@
       <c r="E120">
         <v>2</v>
       </c>
-      <c r="F120">
-        <v>0</v>
+      <c r="F120" t="str">
+        <f t="shared" si="2"/>
+        <v>House</v>
       </c>
       <c r="G120" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H120">
         <v>1</v>
       </c>
       <c r="J120" t="str">
-        <f t="shared" si="1"/>
-        <v>('W5827885', '11 SUNNYBRAE CRES, Toronto, ON', 1199000, 3, 2, 0, 'feras@ucalgary.ca', 1),</v>
+        <f t="shared" si="3"/>
+        <v>('W5827885', '11 SUNNYBRAE CRES, Toronto, ON', 1199000, 3, 2, 'House', 'feras@ucalgary.ca', 1),</v>
       </c>
     </row>
     <row r="121" spans="1:10" x14ac:dyDescent="0.35">
@@ -5065,18 +5184,19 @@
       <c r="E121">
         <v>1</v>
       </c>
-      <c r="F121">
-        <v>0</v>
+      <c r="F121" t="str">
+        <f t="shared" si="2"/>
+        <v>Condo</v>
       </c>
       <c r="G121" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H121">
         <v>2</v>
       </c>
       <c r="J121" t="str">
-        <f t="shared" si="1"/>
-        <v>('C5827921', '#714 629 KING ST, Toronto, ON', 629000, 1, 1, 0, 'feras@ucalgary.ca', 2),</v>
+        <f t="shared" si="3"/>
+        <v>('C5827921', '#714 629 KING ST, Toronto, ON', 629000, 1, 1, 'Condo', 'feras@ucalgary.ca', 2),</v>
       </c>
     </row>
     <row r="122" spans="1:10" x14ac:dyDescent="0.35">
@@ -5095,18 +5215,19 @@
       <c r="E122">
         <v>2</v>
       </c>
-      <c r="F122">
-        <v>0</v>
+      <c r="F122" t="str">
+        <f t="shared" si="2"/>
+        <v>House</v>
       </c>
       <c r="G122" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H122">
         <v>3</v>
       </c>
       <c r="J122" t="str">
-        <f t="shared" si="1"/>
-        <v>('W5827929', '38 VEROBEACH BLVD, Toronto, ON', 848888, 4, 2, 0, 'feras@ucalgary.ca', 3),</v>
+        <f t="shared" si="3"/>
+        <v>('W5827929', '38 VEROBEACH BLVD, Toronto, ON', 848888, 4, 2, 'House', 'feras@ucalgary.ca', 3),</v>
       </c>
     </row>
     <row r="123" spans="1:10" x14ac:dyDescent="0.35">
@@ -5125,18 +5246,19 @@
       <c r="E123">
         <v>4</v>
       </c>
-      <c r="F123">
-        <v>0</v>
+      <c r="F123" t="str">
+        <f t="shared" si="2"/>
+        <v>House</v>
       </c>
       <c r="G123" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H123">
         <v>1</v>
       </c>
       <c r="J123" t="str">
-        <f t="shared" si="1"/>
-        <v>('W5827880', '51 BURNFIELD AVE, Toronto, ON', 2350000, 3, 4, 0, 'feras@ucalgary.ca', 1),</v>
+        <f t="shared" si="3"/>
+        <v>('W5827880', '51 BURNFIELD AVE, Toronto, ON', 2350000, 3, 4, 'House', 'feras@ucalgary.ca', 1),</v>
       </c>
     </row>
     <row r="124" spans="1:10" x14ac:dyDescent="0.35">
@@ -5155,18 +5277,19 @@
       <c r="E124">
         <v>2</v>
       </c>
-      <c r="F124">
-        <v>0</v>
+      <c r="F124" t="str">
+        <f t="shared" si="2"/>
+        <v>Condo</v>
       </c>
       <c r="G124" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H124">
         <v>2</v>
       </c>
       <c r="J124" t="str">
-        <f t="shared" si="1"/>
-        <v>('C5827952', '#ON 2007 HILLCREST AVE, Toronto, ON', 795000, 2, 2, 0, 'feras@ucalgary.ca', 2),</v>
+        <f t="shared" si="3"/>
+        <v>('C5827952', '#ON 2007 HILLCREST AVE, Toronto, ON', 795000, 2, 2, 'Condo', 'feras@ucalgary.ca', 2),</v>
       </c>
     </row>
     <row r="125" spans="1:10" x14ac:dyDescent="0.35">
@@ -5185,18 +5308,19 @@
       <c r="E125">
         <v>2</v>
       </c>
-      <c r="F125">
-        <v>0</v>
+      <c r="F125" t="str">
+        <f t="shared" si="2"/>
+        <v>Condo</v>
       </c>
       <c r="G125" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H125">
         <v>3</v>
       </c>
       <c r="J125" t="str">
-        <f t="shared" si="1"/>
-        <v>('W5827886', '#1012 816 LANSDOWNE AVE, Toronto, ON', 729900, 2, 2, 0, 'feras@ucalgary.ca', 3),</v>
+        <f t="shared" si="3"/>
+        <v>('W5827886', '#1012 816 LANSDOWNE AVE, Toronto, ON', 729900, 2, 2, 'Condo', 'feras@ucalgary.ca', 3),</v>
       </c>
     </row>
     <row r="126" spans="1:10" x14ac:dyDescent="0.35">
@@ -5215,18 +5339,19 @@
       <c r="E126">
         <v>2</v>
       </c>
-      <c r="F126">
-        <v>0</v>
+      <c r="F126" t="str">
+        <f t="shared" si="2"/>
+        <v>Condo</v>
       </c>
       <c r="G126" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H126">
         <v>1</v>
       </c>
       <c r="J126" t="str">
-        <f t="shared" si="1"/>
-        <v>('E5826980', '#304 452 SCARBOROUGH GOLFCLUB RD, Toronto, ON', 408000, 2, 2, 0, 'feras@ucalgary.ca', 1),</v>
+        <f t="shared" si="3"/>
+        <v>('E5826980', '#304 452 SCARBOROUGH GOLFCLUB RD, Toronto, ON', 408000, 2, 2, 'Condo', 'feras@ucalgary.ca', 1),</v>
       </c>
     </row>
     <row r="127" spans="1:10" x14ac:dyDescent="0.35">
@@ -5245,18 +5370,19 @@
       <c r="E127">
         <v>3</v>
       </c>
-      <c r="F127">
-        <v>0</v>
+      <c r="F127" t="str">
+        <f t="shared" si="2"/>
+        <v>House</v>
       </c>
       <c r="G127" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H127">
         <v>2</v>
       </c>
       <c r="J127" t="str">
-        <f t="shared" si="1"/>
-        <v>('C5827246', '#PH05 15 FORT YORK BLVD, Toronto, ON', 3750000, 3, 3, 0, 'feras@ucalgary.ca', 2),</v>
+        <f t="shared" si="3"/>
+        <v>('C5827246', '#PH05 15 FORT YORK BLVD, Toronto, ON', 3750000, 3, 3, 'House', 'feras@ucalgary.ca', 2),</v>
       </c>
     </row>
     <row r="128" spans="1:10" x14ac:dyDescent="0.35">
@@ -5275,18 +5401,19 @@
       <c r="E128">
         <v>5</v>
       </c>
-      <c r="F128">
-        <v>0</v>
+      <c r="F128" t="str">
+        <f t="shared" si="2"/>
+        <v>House</v>
       </c>
       <c r="G128" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H128">
         <v>3</v>
       </c>
       <c r="J128" t="str">
-        <f t="shared" si="1"/>
-        <v>('W5827399', '33 WICKFORD DR, Toronto, ON', 1879000, 5, 5, 0, 'feras@ucalgary.ca', 3),</v>
+        <f t="shared" si="3"/>
+        <v>('W5827399', '33 WICKFORD DR, Toronto, ON', 1879000, 5, 5, 'House', 'feras@ucalgary.ca', 3),</v>
       </c>
     </row>
     <row r="129" spans="1:10" x14ac:dyDescent="0.35">
@@ -5305,18 +5432,19 @@
       <c r="E129">
         <v>3</v>
       </c>
-      <c r="F129">
-        <v>0</v>
+      <c r="F129" t="str">
+        <f t="shared" si="2"/>
+        <v>House</v>
       </c>
       <c r="G129" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H129">
         <v>1</v>
       </c>
       <c r="J129" t="str">
-        <f t="shared" si="1"/>
-        <v>('C5827589', '137 SEATON ST, Toronto, ON', 1780000, 3, 3, 0, 'feras@ucalgary.ca', 1),</v>
+        <f t="shared" si="3"/>
+        <v>('C5827589', '137 SEATON ST, Toronto, ON', 1780000, 3, 3, 'House', 'feras@ucalgary.ca', 1),</v>
       </c>
     </row>
     <row r="130" spans="1:10" x14ac:dyDescent="0.35">
@@ -5335,18 +5463,19 @@
       <c r="E130">
         <v>1</v>
       </c>
-      <c r="F130">
-        <v>0</v>
+      <c r="F130" t="str">
+        <f t="shared" si="2"/>
+        <v>Condo</v>
       </c>
       <c r="G130" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H130">
         <v>2</v>
       </c>
       <c r="J130" t="str">
-        <f t="shared" si="1"/>
-        <v>('E5827590', '411 MAIN ST, Toronto, ON', 599000, 2, 1, 0, 'feras@ucalgary.ca', 2),</v>
+        <f t="shared" si="3"/>
+        <v>('E5827590', '411 MAIN ST, Toronto, ON', 599000, 2, 1, 'Condo', 'feras@ucalgary.ca', 2),</v>
       </c>
     </row>
     <row r="131" spans="1:10" x14ac:dyDescent="0.35">
@@ -5365,18 +5494,19 @@
       <c r="E131">
         <v>2</v>
       </c>
-      <c r="F131">
-        <v>0</v>
+      <c r="F131" t="str">
+        <f t="shared" ref="F131:F188" si="4">IF(D131&lt;3, "Condo", "House")</f>
+        <v>House</v>
       </c>
       <c r="G131" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H131">
         <v>1</v>
       </c>
       <c r="J131" t="str">
-        <f t="shared" ref="J131:J188" si="2">_xlfn.CONCAT("('",A131, "'", ", ", "'", B131, "'", ", ", C131, ", ", D131, ", ", E131, ", ", F131, ", ", "'", G131, "'", ", ", H131, ")", ",")</f>
-        <v>('C5827707', '244 BENSON AVE, Toronto, ON', 1569000, 3, 2, 0, 'feras@ucalgary.ca', 1),</v>
+        <f t="shared" ref="J131:J188" si="5">_xlfn.CONCAT("('",A131, "'", ", ", "'", B131, "'", ", ", C131, ", ", D131, ", ", E131, ", ", "'", F131, "'", ", ", "'", G131, "'", ", ", H131, ")", ",")</f>
+        <v>('C5827707', '244 BENSON AVE, Toronto, ON', 1569000, 3, 2, 'House', 'feras@ucalgary.ca', 1),</v>
       </c>
     </row>
     <row r="132" spans="1:10" x14ac:dyDescent="0.35">
@@ -5395,18 +5525,19 @@
       <c r="E132">
         <v>2</v>
       </c>
-      <c r="F132">
-        <v>0</v>
+      <c r="F132" t="str">
+        <f t="shared" si="4"/>
+        <v>Condo</v>
       </c>
       <c r="G132" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H132">
         <v>2</v>
       </c>
       <c r="J132" t="str">
-        <f t="shared" si="2"/>
-        <v>('C5827219', '#809 70 MILL ST, Toronto, ON', 839000, 2, 2, 0, 'feras@ucalgary.ca', 2),</v>
+        <f t="shared" si="5"/>
+        <v>('C5827219', '#809 70 MILL ST, Toronto, ON', 839000, 2, 2, 'Condo', 'feras@ucalgary.ca', 2),</v>
       </c>
     </row>
     <row r="133" spans="1:10" x14ac:dyDescent="0.35">
@@ -5425,18 +5556,19 @@
       <c r="E133">
         <v>1</v>
       </c>
-      <c r="F133">
-        <v>0</v>
+      <c r="F133" t="str">
+        <f t="shared" si="4"/>
+        <v>Condo</v>
       </c>
       <c r="G133" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H133">
         <v>3</v>
       </c>
       <c r="J133" t="str">
-        <f t="shared" si="2"/>
-        <v>('W5827724', '#213 2772 KEELE ST, Toronto, ON', 499000, 2, 1, 0, 'feras@ucalgary.ca', 3),</v>
+        <f t="shared" si="5"/>
+        <v>('W5827724', '#213 2772 KEELE ST, Toronto, ON', 499000, 2, 1, 'Condo', 'feras@ucalgary.ca', 3),</v>
       </c>
     </row>
     <row r="134" spans="1:10" x14ac:dyDescent="0.35">
@@ -5455,18 +5587,19 @@
       <c r="E134">
         <v>2</v>
       </c>
-      <c r="F134">
-        <v>0</v>
+      <c r="F134" t="str">
+        <f t="shared" si="4"/>
+        <v>Condo</v>
       </c>
       <c r="G134" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H134">
         <v>1</v>
       </c>
       <c r="J134" t="str">
-        <f t="shared" si="2"/>
-        <v>('C5827323', '#1406 10 BELLAIR ST, Toronto, ON', 1539900, 2, 2, 0, 'feras@ucalgary.ca', 1),</v>
+        <f t="shared" si="5"/>
+        <v>('C5827323', '#1406 10 BELLAIR ST, Toronto, ON', 1539900, 2, 2, 'Condo', 'feras@ucalgary.ca', 1),</v>
       </c>
     </row>
     <row r="135" spans="1:10" x14ac:dyDescent="0.35">
@@ -5485,18 +5618,19 @@
       <c r="E135">
         <v>2</v>
       </c>
-      <c r="F135">
-        <v>0</v>
+      <c r="F135" t="str">
+        <f t="shared" si="4"/>
+        <v>Condo</v>
       </c>
       <c r="G135" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H135">
         <v>3</v>
       </c>
       <c r="J135" t="str">
-        <f t="shared" si="2"/>
-        <v>('W5826908', '#213 20 SOUTHPORT ST, Toronto, ON', 569000, 2, 2, 0, 'feras@ucalgary.ca', 3),</v>
+        <f t="shared" si="5"/>
+        <v>('W5826908', '#213 20 SOUTHPORT ST, Toronto, ON', 569000, 2, 2, 'Condo', 'feras@ucalgary.ca', 3),</v>
       </c>
     </row>
     <row r="136" spans="1:10" x14ac:dyDescent="0.35">
@@ -5515,18 +5649,19 @@
       <c r="E136">
         <v>3</v>
       </c>
-      <c r="F136">
-        <v>0</v>
+      <c r="F136" t="str">
+        <f t="shared" si="4"/>
+        <v>House</v>
       </c>
       <c r="G136" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H136">
         <v>1</v>
       </c>
       <c r="J136" t="str">
-        <f t="shared" si="2"/>
-        <v>('W5827909', '3179 IBBETSON CRES, Mississauga, ON', 1100000, 4, 3, 0, 'feras@ucalgary.ca', 1),</v>
+        <f t="shared" si="5"/>
+        <v>('W5827909', '3179 IBBETSON CRES, Mississauga, ON', 1100000, 4, 3, 'House', 'feras@ucalgary.ca', 1),</v>
       </c>
     </row>
     <row r="137" spans="1:10" x14ac:dyDescent="0.35">
@@ -5545,18 +5680,19 @@
       <c r="E137">
         <v>2</v>
       </c>
-      <c r="F137">
-        <v>0</v>
+      <c r="F137" t="str">
+        <f t="shared" si="4"/>
+        <v>House</v>
       </c>
       <c r="G137" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H137">
         <v>2</v>
       </c>
       <c r="J137" t="str">
-        <f t="shared" si="2"/>
-        <v>('W5827928', '#2109 1 VALHALLA INN RD, Toronto, ON', 729900, 3, 2, 0, 'feras@ucalgary.ca', 2),</v>
+        <f t="shared" si="5"/>
+        <v>('W5827928', '#2109 1 VALHALLA INN RD, Toronto, ON', 729900, 3, 2, 'House', 'feras@ucalgary.ca', 2),</v>
       </c>
     </row>
     <row r="138" spans="1:10" x14ac:dyDescent="0.35">
@@ -5575,18 +5711,19 @@
       <c r="E138">
         <v>4</v>
       </c>
-      <c r="F138">
-        <v>0</v>
+      <c r="F138" t="str">
+        <f t="shared" si="4"/>
+        <v>House</v>
       </c>
       <c r="G138" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H138">
         <v>3</v>
       </c>
       <c r="J138" t="str">
-        <f t="shared" si="2"/>
-        <v>('W5827892', '38 ROYAL VISTA RD, Brampton, ON', 915000, 4, 4, 0, 'feras@ucalgary.ca', 3),</v>
+        <f t="shared" si="5"/>
+        <v>('W5827892', '38 ROYAL VISTA RD, Brampton, ON', 915000, 4, 4, 'House', 'feras@ucalgary.ca', 3),</v>
       </c>
     </row>
     <row r="139" spans="1:10" x14ac:dyDescent="0.35">
@@ -5605,18 +5742,19 @@
       <c r="E139">
         <v>3</v>
       </c>
-      <c r="F139">
-        <v>0</v>
+      <c r="F139" t="str">
+        <f t="shared" si="4"/>
+        <v>House</v>
       </c>
       <c r="G139" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H139">
         <v>1</v>
       </c>
       <c r="J139" t="str">
-        <f t="shared" si="2"/>
-        <v>('W5827911', '80A CORBY CRES, Brampton, ON', 699000, 3, 3, 0, 'feras@ucalgary.ca', 1),</v>
+        <f t="shared" si="5"/>
+        <v>('W5827911', '80A CORBY CRES, Brampton, ON', 699000, 3, 3, 'House', 'feras@ucalgary.ca', 1),</v>
       </c>
     </row>
     <row r="140" spans="1:10" x14ac:dyDescent="0.35">
@@ -5635,18 +5773,19 @@
       <c r="E140">
         <v>2</v>
       </c>
-      <c r="F140">
-        <v>0</v>
+      <c r="F140" t="str">
+        <f t="shared" si="4"/>
+        <v>House</v>
       </c>
       <c r="G140" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H140">
         <v>2</v>
       </c>
       <c r="J140" t="str">
-        <f t="shared" si="2"/>
-        <v>('W5827935', '50 ERINGATE DR, Toronto, ON', 949000, 3, 2, 0, 'feras@ucalgary.ca', 2),</v>
+        <f t="shared" si="5"/>
+        <v>('W5827935', '50 ERINGATE DR, Toronto, ON', 949000, 3, 2, 'House', 'feras@ucalgary.ca', 2),</v>
       </c>
     </row>
     <row r="141" spans="1:10" x14ac:dyDescent="0.35">
@@ -5665,18 +5804,19 @@
       <c r="E141">
         <v>4</v>
       </c>
-      <c r="F141">
-        <v>0</v>
+      <c r="F141" t="str">
+        <f t="shared" si="4"/>
+        <v>House</v>
       </c>
       <c r="G141" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H141">
         <v>1</v>
       </c>
       <c r="J141" t="str">
-        <f t="shared" si="2"/>
-        <v>('W5827400', '3259 SCOTCH PINE GATE AVE, Mississauga, ON', 1259000, 5, 4, 0, 'feras@ucalgary.ca', 1),</v>
+        <f t="shared" si="5"/>
+        <v>('W5827400', '3259 SCOTCH PINE GATE AVE, Mississauga, ON', 1259000, 5, 4, 'House', 'feras@ucalgary.ca', 1),</v>
       </c>
     </row>
     <row r="142" spans="1:10" x14ac:dyDescent="0.35">
@@ -5695,18 +5835,19 @@
       <c r="E142">
         <v>3</v>
       </c>
-      <c r="F142">
-        <v>0</v>
+      <c r="F142" t="str">
+        <f t="shared" si="4"/>
+        <v>House</v>
       </c>
       <c r="G142" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H142">
         <v>2</v>
       </c>
       <c r="J142" t="str">
-        <f t="shared" si="2"/>
-        <v>('40349553', '1457 WAKEHURST Crescent, Oakville, ON', 1479000, 4, 3, 0, 'feras@ucalgary.ca', 2),</v>
+        <f t="shared" si="5"/>
+        <v>('40349553', '1457 WAKEHURST Crescent, Oakville, ON', 1479000, 4, 3, 'House', 'feras@ucalgary.ca', 2),</v>
       </c>
     </row>
     <row r="143" spans="1:10" x14ac:dyDescent="0.35">
@@ -5725,18 +5866,19 @@
       <c r="E143">
         <v>2</v>
       </c>
-      <c r="F143">
-        <v>0</v>
+      <c r="F143" t="str">
+        <f t="shared" si="4"/>
+        <v>Condo</v>
       </c>
       <c r="G143" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H143">
         <v>3</v>
       </c>
       <c r="J143" t="str">
-        <f t="shared" si="2"/>
-        <v>('W5827557', '#3203 208 ENFIELD PL, Mississauga, ON', 736888, 2, 2, 0, 'feras@ucalgary.ca', 3),</v>
+        <f t="shared" si="5"/>
+        <v>('W5827557', '#3203 208 ENFIELD PL, Mississauga, ON', 736888, 2, 2, 'Condo', 'feras@ucalgary.ca', 3),</v>
       </c>
     </row>
     <row r="144" spans="1:10" x14ac:dyDescent="0.35">
@@ -5755,18 +5897,19 @@
       <c r="E144">
         <v>2</v>
       </c>
-      <c r="F144">
-        <v>0</v>
+      <c r="F144" t="str">
+        <f t="shared" si="4"/>
+        <v>Condo</v>
       </c>
       <c r="G144" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H144">
         <v>2</v>
       </c>
       <c r="J144" t="str">
-        <f t="shared" si="2"/>
-        <v>('40349719', '4085 PARKSIDE VILLAGE Drive Unit# 310, Mississauga, ON', 749900, 2, 2, 0, 'feras@ucalgary.ca', 2),</v>
+        <f t="shared" si="5"/>
+        <v>('40349719', '4085 PARKSIDE VILLAGE Drive Unit# 310, Mississauga, ON', 749900, 2, 2, 'Condo', 'feras@ucalgary.ca', 2),</v>
       </c>
     </row>
     <row r="145" spans="1:10" x14ac:dyDescent="0.35">
@@ -5785,18 +5928,19 @@
       <c r="E145">
         <v>3</v>
       </c>
-      <c r="F145">
-        <v>0</v>
+      <c r="F145" t="str">
+        <f t="shared" si="4"/>
+        <v>House</v>
       </c>
       <c r="G145" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H145">
         <v>3</v>
       </c>
       <c r="J145" t="str">
-        <f t="shared" si="2"/>
-        <v>('W5826905', '938 BLAIRHOLM AVE, Mississauga, ON', 999000, 4, 3, 0, 'feras@ucalgary.ca', 3),</v>
+        <f t="shared" si="5"/>
+        <v>('W5826905', '938 BLAIRHOLM AVE, Mississauga, ON', 999000, 4, 3, 'House', 'feras@ucalgary.ca', 3),</v>
       </c>
     </row>
     <row r="146" spans="1:10" x14ac:dyDescent="0.35">
@@ -5815,18 +5959,19 @@
       <c r="E146">
         <v>5</v>
       </c>
-      <c r="F146">
-        <v>0</v>
+      <c r="F146" t="str">
+        <f t="shared" si="4"/>
+        <v>House</v>
       </c>
       <c r="G146" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H146">
         <v>2</v>
       </c>
       <c r="J146" t="str">
-        <f t="shared" si="2"/>
-        <v>('W5826834', '1425 CHRISEDEN DR, Mississauga, ON', 4125000, 4, 5, 0, 'feras@ucalgary.ca', 2),</v>
+        <f t="shared" si="5"/>
+        <v>('W5826834', '1425 CHRISEDEN DR, Mississauga, ON', 4125000, 4, 5, 'House', 'feras@ucalgary.ca', 2),</v>
       </c>
     </row>
     <row r="147" spans="1:10" x14ac:dyDescent="0.35">
@@ -5845,18 +5990,19 @@
       <c r="E147">
         <v>4</v>
       </c>
-      <c r="F147">
-        <v>0</v>
+      <c r="F147" t="str">
+        <f t="shared" si="4"/>
+        <v>House</v>
       </c>
       <c r="G147" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H147">
         <v>3</v>
       </c>
       <c r="J147" t="str">
-        <f t="shared" si="2"/>
-        <v>('W5827351', '128 PARK ST E, Mississauga, ON', 1219000, 3, 4, 0, 'feras@ucalgary.ca', 3),</v>
+        <f t="shared" si="5"/>
+        <v>('W5827351', '128 PARK ST E, Mississauga, ON', 1219000, 3, 4, 'House', 'feras@ucalgary.ca', 3),</v>
       </c>
     </row>
     <row r="148" spans="1:10" x14ac:dyDescent="0.35">
@@ -5875,18 +6021,19 @@
       <c r="E148">
         <v>3</v>
       </c>
-      <c r="F148">
-        <v>0</v>
+      <c r="F148" t="str">
+        <f t="shared" si="4"/>
+        <v>House</v>
       </c>
       <c r="G148" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H148">
         <v>1</v>
       </c>
       <c r="J148" t="str">
-        <f t="shared" si="2"/>
-        <v>('W5827448', '63 VIVIANS CRES, Brampton, ON', 1024990, 3, 3, 0, 'feras@ucalgary.ca', 1),</v>
+        <f t="shared" si="5"/>
+        <v>('W5827448', '63 VIVIANS CRES, Brampton, ON', 1024990, 3, 3, 'House', 'feras@ucalgary.ca', 1),</v>
       </c>
     </row>
     <row r="149" spans="1:10" x14ac:dyDescent="0.35">
@@ -5905,18 +6052,19 @@
       <c r="E149">
         <v>2</v>
       </c>
-      <c r="F149">
-        <v>0</v>
+      <c r="F149" t="str">
+        <f t="shared" si="4"/>
+        <v>Condo</v>
       </c>
       <c r="G149" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H149">
         <v>2</v>
       </c>
       <c r="J149" t="str">
-        <f t="shared" si="2"/>
-        <v>('H4151093', '80 ABSOLUTE Avenue Unit #311, Mississauga, ON', 569420, 1, 2, 0, 'feras@ucalgary.ca', 2),</v>
+        <f t="shared" si="5"/>
+        <v>('H4151093', '80 ABSOLUTE Avenue Unit #311, Mississauga, ON', 569420, 1, 2, 'Condo', 'feras@ucalgary.ca', 2),</v>
       </c>
     </row>
     <row r="150" spans="1:10" x14ac:dyDescent="0.35">
@@ -5935,18 +6083,19 @@
       <c r="E150">
         <v>2</v>
       </c>
-      <c r="F150">
-        <v>0</v>
+      <c r="F150" t="str">
+        <f t="shared" si="4"/>
+        <v>House</v>
       </c>
       <c r="G150" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H150">
         <v>3</v>
       </c>
       <c r="J150" t="str">
-        <f t="shared" si="2"/>
-        <v>('40349185', '53 RAYSIDE Drive, Etobicoke, ON', 1199919, 5, 2, 0, 'feras@ucalgary.ca', 3),</v>
+        <f t="shared" si="5"/>
+        <v>('40349185', '53 RAYSIDE Drive, Etobicoke, ON', 1199919, 5, 2, 'House', 'feras@ucalgary.ca', 3),</v>
       </c>
     </row>
     <row r="151" spans="1:10" x14ac:dyDescent="0.35">
@@ -5965,18 +6114,19 @@
       <c r="E151">
         <v>4</v>
       </c>
-      <c r="F151">
-        <v>0</v>
+      <c r="F151" t="str">
+        <f t="shared" si="4"/>
+        <v>House</v>
       </c>
       <c r="G151" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H151">
         <v>1</v>
       </c>
       <c r="J151" t="str">
-        <f t="shared" si="2"/>
-        <v>('W5826874', '52A TREEVIEW DR, Toronto, ON', 1428800, 4, 4, 0, 'feras@ucalgary.ca', 1),</v>
+        <f t="shared" si="5"/>
+        <v>('W5826874', '52A TREEVIEW DR, Toronto, ON', 1428800, 4, 4, 'House', 'feras@ucalgary.ca', 1),</v>
       </c>
     </row>
     <row r="152" spans="1:10" x14ac:dyDescent="0.35">
@@ -5995,18 +6145,19 @@
       <c r="E152">
         <v>3</v>
       </c>
-      <c r="F152">
-        <v>0</v>
+      <c r="F152" t="str">
+        <f t="shared" si="4"/>
+        <v>House</v>
       </c>
       <c r="G152" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H152">
         <v>2</v>
       </c>
       <c r="J152" t="str">
-        <f t="shared" si="2"/>
-        <v>('W5827446', '11 ROSEMEADE AVE, Toronto, ON', 1349900, 5, 3, 0, 'feras@ucalgary.ca', 2),</v>
+        <f t="shared" si="5"/>
+        <v>('W5827446', '11 ROSEMEADE AVE, Toronto, ON', 1349900, 5, 3, 'House', 'feras@ucalgary.ca', 2),</v>
       </c>
     </row>
     <row r="153" spans="1:10" x14ac:dyDescent="0.35">
@@ -6025,18 +6176,19 @@
       <c r="E153">
         <v>2</v>
       </c>
-      <c r="F153">
-        <v>0</v>
+      <c r="F153" t="str">
+        <f t="shared" si="4"/>
+        <v>Condo</v>
       </c>
       <c r="G153" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H153">
         <v>3</v>
       </c>
       <c r="J153" t="str">
-        <f t="shared" si="2"/>
-        <v>('R2738552', '208 8070 OAK STREET, Vancouver, BC', 1179700, 2, 2, 0, 'feras@ucalgary.ca', 3),</v>
+        <f t="shared" si="5"/>
+        <v>('R2738552', '208 8070 OAK STREET, Vancouver, BC', 1179700, 2, 2, 'Condo', 'feras@ucalgary.ca', 3),</v>
       </c>
     </row>
     <row r="154" spans="1:10" x14ac:dyDescent="0.35">
@@ -6055,18 +6207,19 @@
       <c r="E154">
         <v>2</v>
       </c>
-      <c r="F154">
-        <v>0</v>
+      <c r="F154" t="str">
+        <f t="shared" si="4"/>
+        <v>Condo</v>
       </c>
       <c r="G154" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H154">
         <v>1</v>
       </c>
       <c r="J154" t="str">
-        <f t="shared" si="2"/>
-        <v>('R2738530', '1106 5629 BIRNEY AVENUE, Vancouver, BC', 1319000, 2, 2, 0, 'feras@ucalgary.ca', 1),</v>
+        <f t="shared" si="5"/>
+        <v>('R2738530', '1106 5629 BIRNEY AVENUE, Vancouver, BC', 1319000, 2, 2, 'Condo', 'feras@ucalgary.ca', 1),</v>
       </c>
     </row>
     <row r="155" spans="1:10" x14ac:dyDescent="0.35">
@@ -6085,18 +6238,19 @@
       <c r="E155">
         <v>3</v>
       </c>
-      <c r="F155">
-        <v>0</v>
+      <c r="F155" t="str">
+        <f t="shared" si="4"/>
+        <v>House</v>
       </c>
       <c r="G155" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H155">
         <v>2</v>
       </c>
       <c r="J155" t="str">
-        <f t="shared" si="2"/>
-        <v>('R2738528', '1278 DUCHESS AVENUE, West Vancouver, BC', 2198000, 3, 3, 0, 'feras@ucalgary.ca', 2),</v>
+        <f t="shared" si="5"/>
+        <v>('R2738528', '1278 DUCHESS AVENUE, West Vancouver, BC', 2198000, 3, 3, 'House', 'feras@ucalgary.ca', 2),</v>
       </c>
     </row>
     <row r="156" spans="1:10" x14ac:dyDescent="0.35">
@@ -6115,18 +6269,19 @@
       <c r="E156">
         <v>5</v>
       </c>
-      <c r="F156">
-        <v>0</v>
+      <c r="F156" t="str">
+        <f t="shared" si="4"/>
+        <v>House</v>
       </c>
       <c r="G156" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H156">
         <v>3</v>
       </c>
       <c r="J156" t="str">
-        <f t="shared" si="2"/>
-        <v>('R2738554', '3206 CAROLINA STREET, Vancouver, BC', 2198000, 6, 5, 0, 'feras@ucalgary.ca', 3),</v>
+        <f t="shared" si="5"/>
+        <v>('R2738554', '3206 CAROLINA STREET, Vancouver, BC', 2198000, 6, 5, 'House', 'feras@ucalgary.ca', 3),</v>
       </c>
     </row>
     <row r="157" spans="1:10" x14ac:dyDescent="0.35">
@@ -6145,18 +6300,19 @@
       <c r="E157">
         <v>2</v>
       </c>
-      <c r="F157">
-        <v>0</v>
+      <c r="F157" t="str">
+        <f t="shared" si="4"/>
+        <v>Condo</v>
       </c>
       <c r="G157" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H157">
         <v>1</v>
       </c>
       <c r="J157" t="str">
-        <f t="shared" si="2"/>
-        <v>('R2738518', '2005 4388 BUCHANAN STREET, Burnaby, BC', 849900, 2, 2, 0, 'feras@ucalgary.ca', 1),</v>
+        <f t="shared" si="5"/>
+        <v>('R2738518', '2005 4388 BUCHANAN STREET, Burnaby, BC', 849900, 2, 2, 'Condo', 'feras@ucalgary.ca', 1),</v>
       </c>
     </row>
     <row r="158" spans="1:10" x14ac:dyDescent="0.35">
@@ -6175,18 +6331,19 @@
       <c r="E158">
         <v>1</v>
       </c>
-      <c r="F158">
-        <v>0</v>
+      <c r="F158" t="str">
+        <f t="shared" si="4"/>
+        <v>Condo</v>
       </c>
       <c r="G158" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H158">
         <v>2</v>
       </c>
       <c r="J158" t="str">
-        <f t="shared" si="2"/>
-        <v>('R2738548', '201 8070 OAK STREET, Vancouver, BC', 917700, 1, 1, 0, 'feras@ucalgary.ca', 2),</v>
+        <f t="shared" si="5"/>
+        <v>('R2738548', '201 8070 OAK STREET, Vancouver, BC', 917700, 1, 1, 'Condo', 'feras@ucalgary.ca', 2),</v>
       </c>
     </row>
     <row r="159" spans="1:10" x14ac:dyDescent="0.35">
@@ -6205,18 +6362,19 @@
       <c r="E159">
         <v>2</v>
       </c>
-      <c r="F159">
-        <v>0</v>
+      <c r="F159" t="str">
+        <f t="shared" si="4"/>
+        <v>House</v>
       </c>
       <c r="G159" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H159">
         <v>3</v>
       </c>
       <c r="J159" t="str">
-        <f t="shared" si="2"/>
-        <v>('R2738556', '202 8030 OAK STREET, Vancouver, BC', 1379800, 3, 2, 0, 'feras@ucalgary.ca', 3),</v>
+        <f t="shared" si="5"/>
+        <v>('R2738556', '202 8030 OAK STREET, Vancouver, BC', 1379800, 3, 2, 'House', 'feras@ucalgary.ca', 3),</v>
       </c>
     </row>
     <row r="160" spans="1:10" x14ac:dyDescent="0.35">
@@ -6235,18 +6393,19 @@
       <c r="E160">
         <v>1</v>
       </c>
-      <c r="F160">
-        <v>0</v>
+      <c r="F160" t="str">
+        <f t="shared" si="4"/>
+        <v>Condo</v>
       </c>
       <c r="G160" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H160">
         <v>1</v>
       </c>
       <c r="J160" t="str">
-        <f t="shared" si="2"/>
-        <v>('R2738581', '605 53 W HASTINGS STREET, Vancouver, BC', 875000, 1, 1, 0, 'feras@ucalgary.ca', 1),</v>
+        <f t="shared" si="5"/>
+        <v>('R2738581', '605 53 W HASTINGS STREET, Vancouver, BC', 875000, 1, 1, 'Condo', 'feras@ucalgary.ca', 1),</v>
       </c>
     </row>
     <row r="161" spans="1:10" x14ac:dyDescent="0.35">
@@ -6265,18 +6424,19 @@
       <c r="E161">
         <v>1</v>
       </c>
-      <c r="F161">
-        <v>0</v>
+      <c r="F161" t="str">
+        <f t="shared" si="4"/>
+        <v>Condo</v>
       </c>
       <c r="G161" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H161">
         <v>2</v>
       </c>
       <c r="J161" t="str">
-        <f t="shared" si="2"/>
-        <v>('R2738546', '102 8030 OAK STREET, Vancouver, BC', 698800, 1, 1, 0, 'feras@ucalgary.ca', 2),</v>
+        <f t="shared" si="5"/>
+        <v>('R2738546', '102 8030 OAK STREET, Vancouver, BC', 698800, 1, 1, 'Condo', 'feras@ucalgary.ca', 2),</v>
       </c>
     </row>
     <row r="162" spans="1:10" x14ac:dyDescent="0.35">
@@ -6295,18 +6455,19 @@
       <c r="E162">
         <v>5</v>
       </c>
-      <c r="F162">
-        <v>0</v>
+      <c r="F162" t="str">
+        <f t="shared" si="4"/>
+        <v>House</v>
       </c>
       <c r="G162" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H162">
         <v>3</v>
       </c>
       <c r="J162" t="str">
-        <f t="shared" si="2"/>
-        <v>('R2738543', '3206 CAROLINA STREET, Vancouver, BC', 2198000, 6, 5, 0, 'feras@ucalgary.ca', 3),</v>
+        <f t="shared" si="5"/>
+        <v>('R2738543', '3206 CAROLINA STREET, Vancouver, BC', 2198000, 6, 5, 'House', 'feras@ucalgary.ca', 3),</v>
       </c>
     </row>
     <row r="163" spans="1:10" x14ac:dyDescent="0.35">
@@ -6325,18 +6486,19 @@
       <c r="E163">
         <v>2</v>
       </c>
-      <c r="F163">
-        <v>0</v>
+      <c r="F163" t="str">
+        <f t="shared" si="4"/>
+        <v>House</v>
       </c>
       <c r="G163" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H163">
         <v>1</v>
       </c>
       <c r="J163" t="str">
-        <f t="shared" si="2"/>
-        <v>('R2738527', '167 2035 GLENAIRE DRIVE, North Vancouver, BC', 1159000, 3, 2, 0, 'feras@ucalgary.ca', 1),</v>
+        <f t="shared" si="5"/>
+        <v>('R2738527', '167 2035 GLENAIRE DRIVE, North Vancouver, BC', 1159000, 3, 2, 'House', 'feras@ucalgary.ca', 1),</v>
       </c>
     </row>
     <row r="164" spans="1:10" x14ac:dyDescent="0.35">
@@ -6355,18 +6517,19 @@
       <c r="E164">
         <v>3</v>
       </c>
-      <c r="F164">
-        <v>0</v>
+      <c r="F164" t="str">
+        <f t="shared" si="4"/>
+        <v>House</v>
       </c>
       <c r="G164" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H164">
         <v>2</v>
       </c>
       <c r="J164" t="str">
-        <f t="shared" si="2"/>
-        <v>('X5826720', '3616 POINT GREY RD, Vancouver, BC', 4880000, 4, 3, 0, 'feras@ucalgary.ca', 2),</v>
+        <f t="shared" si="5"/>
+        <v>('X5826720', '3616 POINT GREY RD, Vancouver, BC', 4880000, 4, 3, 'House', 'feras@ucalgary.ca', 2),</v>
       </c>
     </row>
     <row r="165" spans="1:10" x14ac:dyDescent="0.35">
@@ -6385,18 +6548,19 @@
       <c r="E165">
         <v>5</v>
       </c>
-      <c r="F165">
-        <v>0</v>
+      <c r="F165" t="str">
+        <f t="shared" si="4"/>
+        <v>House</v>
       </c>
       <c r="G165" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H165">
         <v>3</v>
       </c>
       <c r="J165" t="str">
-        <f t="shared" si="2"/>
-        <v>('R2738231', 'PH1 1550 ALBERNI STREET, Vancouver, BC', 31880800, 3, 5, 0, 'feras@ucalgary.ca', 3),</v>
+        <f t="shared" si="5"/>
+        <v>('R2738231', 'PH1 1550 ALBERNI STREET, Vancouver, BC', 31880800, 3, 5, 'House', 'feras@ucalgary.ca', 3),</v>
       </c>
     </row>
     <row r="166" spans="1:10" x14ac:dyDescent="0.35">
@@ -6415,18 +6579,19 @@
       <c r="E166">
         <v>3</v>
       </c>
-      <c r="F166">
-        <v>0</v>
+      <c r="F166" t="str">
+        <f t="shared" si="4"/>
+        <v>House</v>
       </c>
       <c r="G166" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H166">
         <v>1</v>
       </c>
       <c r="J166" t="str">
-        <f t="shared" si="2"/>
-        <v>('R2738215', '3403 1189 MELVILLE STREET, Vancouver, BC', 2848000, 3, 3, 0, 'feras@ucalgary.ca', 1),</v>
+        <f t="shared" si="5"/>
+        <v>('R2738215', '3403 1189 MELVILLE STREET, Vancouver, BC', 2848000, 3, 3, 'House', 'feras@ucalgary.ca', 1),</v>
       </c>
     </row>
     <row r="167" spans="1:10" x14ac:dyDescent="0.35">
@@ -6445,18 +6610,19 @@
       <c r="E167">
         <v>2</v>
       </c>
-      <c r="F167">
-        <v>0</v>
+      <c r="F167" t="str">
+        <f t="shared" si="4"/>
+        <v>Condo</v>
       </c>
       <c r="G167" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H167">
         <v>2</v>
       </c>
       <c r="J167" t="str">
-        <f t="shared" si="2"/>
-        <v>('R2738301', '204 565 17TH STREET, West Vancouver, BC', 1150000, 2, 2, 0, 'feras@ucalgary.ca', 2),</v>
+        <f t="shared" si="5"/>
+        <v>('R2738301', '204 565 17TH STREET, West Vancouver, BC', 1150000, 2, 2, 'Condo', 'feras@ucalgary.ca', 2),</v>
       </c>
     </row>
     <row r="168" spans="1:10" x14ac:dyDescent="0.35">
@@ -6475,18 +6641,19 @@
       <c r="E168">
         <v>2</v>
       </c>
-      <c r="F168">
-        <v>0</v>
+      <c r="F168" t="str">
+        <f t="shared" si="4"/>
+        <v>Condo</v>
       </c>
       <c r="G168" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H168">
         <v>3</v>
       </c>
       <c r="J168" t="str">
-        <f t="shared" si="2"/>
-        <v>('R2738168', '1403 1818 ALBERNI STREET, Vancouver, BC', 2269900, 2, 2, 0, 'feras@ucalgary.ca', 3),</v>
+        <f t="shared" si="5"/>
+        <v>('R2738168', '1403 1818 ALBERNI STREET, Vancouver, BC', 2269900, 2, 2, 'Condo', 'feras@ucalgary.ca', 3),</v>
       </c>
     </row>
     <row r="169" spans="1:10" x14ac:dyDescent="0.35">
@@ -6505,18 +6672,19 @@
       <c r="E169">
         <v>2</v>
       </c>
-      <c r="F169">
-        <v>0</v>
+      <c r="F169" t="str">
+        <f t="shared" si="4"/>
+        <v>Condo</v>
       </c>
       <c r="G169" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H169">
         <v>1</v>
       </c>
       <c r="J169" t="str">
-        <f t="shared" si="2"/>
-        <v>('R2738296', '2002 1550 FERN STREET, North Vancouver, BC', 924000, 2, 2, 0, 'feras@ucalgary.ca', 1),</v>
+        <f t="shared" si="5"/>
+        <v>('R2738296', '2002 1550 FERN STREET, North Vancouver, BC', 924000, 2, 2, 'Condo', 'feras@ucalgary.ca', 1),</v>
       </c>
     </row>
     <row r="170" spans="1:10" x14ac:dyDescent="0.35">
@@ -6535,18 +6703,19 @@
       <c r="E170">
         <v>2</v>
       </c>
-      <c r="F170">
-        <v>0</v>
+      <c r="F170" t="str">
+        <f t="shared" si="4"/>
+        <v>Condo</v>
       </c>
       <c r="G170" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H170">
         <v>2</v>
       </c>
       <c r="J170" t="str">
-        <f t="shared" si="2"/>
-        <v>('R2738293', '101 5615 HAMPTON PLACE, Vancouver, BC', 1050000, 2, 2, 0, 'feras@ucalgary.ca', 2),</v>
+        <f t="shared" si="5"/>
+        <v>('R2738293', '101 5615 HAMPTON PLACE, Vancouver, BC', 1050000, 2, 2, 'Condo', 'feras@ucalgary.ca', 2),</v>
       </c>
     </row>
     <row r="171" spans="1:10" x14ac:dyDescent="0.35">
@@ -6565,18 +6734,19 @@
       <c r="E171">
         <v>1</v>
       </c>
-      <c r="F171">
-        <v>0</v>
+      <c r="F171" t="str">
+        <f t="shared" si="4"/>
+        <v>Condo</v>
       </c>
       <c r="G171" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H171">
         <v>3</v>
       </c>
       <c r="J171" t="str">
-        <f t="shared" si="2"/>
-        <v>('202226988', '13 Hull Avenue, Winnipeg, MB', 349900, 2, 1, 0, 'feras@ucalgary.ca', 3),</v>
+        <f t="shared" si="5"/>
+        <v>('202226988', '13 Hull Avenue, Winnipeg, MB', 349900, 2, 1, 'Condo', 'feras@ucalgary.ca', 3),</v>
       </c>
     </row>
     <row r="172" spans="1:10" x14ac:dyDescent="0.35">
@@ -6595,18 +6765,19 @@
       <c r="E172">
         <v>3</v>
       </c>
-      <c r="F172">
-        <v>0</v>
+      <c r="F172" t="str">
+        <f t="shared" si="4"/>
+        <v>House</v>
       </c>
       <c r="G172" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H172">
         <v>1</v>
       </c>
       <c r="J172" t="str">
-        <f t="shared" si="2"/>
-        <v>('202227043', '190 Springwater Road, Winnipeg, MB', 674900, 3, 3, 0, 'feras@ucalgary.ca', 1),</v>
+        <f t="shared" si="5"/>
+        <v>('202227043', '190 Springwater Road, Winnipeg, MB', 674900, 3, 3, 'House', 'feras@ucalgary.ca', 1),</v>
       </c>
     </row>
     <row r="173" spans="1:10" x14ac:dyDescent="0.35">
@@ -6625,18 +6796,19 @@
       <c r="E173">
         <v>2</v>
       </c>
-      <c r="F173">
-        <v>0</v>
+      <c r="F173" t="str">
+        <f t="shared" si="4"/>
+        <v>House</v>
       </c>
       <c r="G173" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H173">
         <v>2</v>
       </c>
       <c r="J173" t="str">
-        <f t="shared" si="2"/>
-        <v>('202227027', '475 Besant Street, Winnipeg, MB', 349000, 4, 2, 0, 'feras@ucalgary.ca', 2),</v>
+        <f t="shared" si="5"/>
+        <v>('202227027', '475 Besant Street, Winnipeg, MB', 349000, 4, 2, 'House', 'feras@ucalgary.ca', 2),</v>
       </c>
     </row>
     <row r="174" spans="1:10" x14ac:dyDescent="0.35">
@@ -6655,18 +6827,19 @@
       <c r="E174">
         <v>1</v>
       </c>
-      <c r="F174">
-        <v>0</v>
+      <c r="F174" t="str">
+        <f t="shared" si="4"/>
+        <v>House</v>
       </c>
       <c r="G174" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H174">
         <v>3</v>
       </c>
       <c r="J174" t="str">
-        <f t="shared" si="2"/>
-        <v>('202227046', '669 Alfred Avenue, Winnipeg, MB', 169900, 3, 1, 0, 'feras@ucalgary.ca', 3),</v>
+        <f t="shared" si="5"/>
+        <v>('202227046', '669 Alfred Avenue, Winnipeg, MB', 169900, 3, 1, 'House', 'feras@ucalgary.ca', 3),</v>
       </c>
     </row>
     <row r="175" spans="1:10" x14ac:dyDescent="0.35">
@@ -6685,18 +6858,19 @@
       <c r="E175">
         <v>1</v>
       </c>
-      <c r="F175">
-        <v>0</v>
+      <c r="F175" t="str">
+        <f t="shared" si="4"/>
+        <v>Condo</v>
       </c>
       <c r="G175" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H175">
         <v>1</v>
       </c>
       <c r="J175" t="str">
-        <f t="shared" si="2"/>
-        <v>('202224448', '38 Inman Avenue, Winnipeg, MB', 270000, 2, 1, 0, 'feras@ucalgary.ca', 1),</v>
+        <f t="shared" si="5"/>
+        <v>('202224448', '38 Inman Avenue, Winnipeg, MB', 270000, 2, 1, 'Condo', 'feras@ucalgary.ca', 1),</v>
       </c>
     </row>
     <row r="176" spans="1:10" x14ac:dyDescent="0.35">
@@ -6715,18 +6889,19 @@
       <c r="E176">
         <v>3</v>
       </c>
-      <c r="F176">
-        <v>0</v>
+      <c r="F176" t="str">
+        <f t="shared" si="4"/>
+        <v>House</v>
       </c>
       <c r="G176" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H176">
         <v>2</v>
       </c>
       <c r="J176" t="str">
-        <f t="shared" si="2"/>
-        <v>('202226958', '32 SOUTHLANDS Drive, East St Paul, MB', 1057000, 5, 3, 0, 'feras@ucalgary.ca', 2),</v>
+        <f t="shared" si="5"/>
+        <v>('202226958', '32 SOUTHLANDS Drive, East St Paul, MB', 1057000, 5, 3, 'House', 'feras@ucalgary.ca', 2),</v>
       </c>
     </row>
     <row r="177" spans="1:10" x14ac:dyDescent="0.35">
@@ -6745,18 +6920,19 @@
       <c r="E177">
         <v>2</v>
       </c>
-      <c r="F177">
-        <v>0</v>
+      <c r="F177" t="str">
+        <f t="shared" si="4"/>
+        <v>House</v>
       </c>
       <c r="G177" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H177">
         <v>3</v>
       </c>
       <c r="J177" t="str">
-        <f t="shared" si="2"/>
-        <v>('202226877', '55 Forestgate Avenue, Winnipeg, MB', 499000, 3, 2, 0, 'feras@ucalgary.ca', 3),</v>
+        <f t="shared" si="5"/>
+        <v>('202226877', '55 Forestgate Avenue, Winnipeg, MB', 499000, 3, 2, 'House', 'feras@ucalgary.ca', 3),</v>
       </c>
     </row>
     <row r="178" spans="1:10" x14ac:dyDescent="0.35">
@@ -6775,18 +6951,19 @@
       <c r="E178">
         <v>1</v>
       </c>
-      <c r="F178">
-        <v>0</v>
+      <c r="F178" t="str">
+        <f t="shared" si="4"/>
+        <v>Condo</v>
       </c>
       <c r="G178" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H178">
         <v>1</v>
       </c>
       <c r="J178" t="str">
-        <f t="shared" si="2"/>
-        <v>('202226999', '32 Crystal Avenue, Winnipeg, MB', 198700, 2, 1, 0, 'feras@ucalgary.ca', 1),</v>
+        <f t="shared" si="5"/>
+        <v>('202226999', '32 Crystal Avenue, Winnipeg, MB', 198700, 2, 1, 'Condo', 'feras@ucalgary.ca', 1),</v>
       </c>
     </row>
     <row r="179" spans="1:10" x14ac:dyDescent="0.35">
@@ -6805,18 +6982,19 @@
       <c r="E179">
         <v>1</v>
       </c>
-      <c r="F179">
-        <v>0</v>
+      <c r="F179" t="str">
+        <f t="shared" si="4"/>
+        <v>Condo</v>
       </c>
       <c r="G179" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H179">
         <v>2</v>
       </c>
       <c r="J179" t="str">
-        <f t="shared" si="2"/>
-        <v>('202227009', '206 Yale Avenue, Winnipeg, MB', 229900, 2, 1, 0, 'feras@ucalgary.ca', 2),</v>
+        <f t="shared" si="5"/>
+        <v>('202227009', '206 Yale Avenue, Winnipeg, MB', 229900, 2, 1, 'Condo', 'feras@ucalgary.ca', 2),</v>
       </c>
     </row>
     <row r="180" spans="1:10" x14ac:dyDescent="0.35">
@@ -6835,18 +7013,19 @@
       <c r="E180">
         <v>3</v>
       </c>
-      <c r="F180">
-        <v>0</v>
+      <c r="F180" t="str">
+        <f t="shared" si="4"/>
+        <v>House</v>
       </c>
       <c r="G180" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H180">
         <v>1</v>
       </c>
       <c r="J180" t="str">
-        <f t="shared" si="2"/>
-        <v>('202226895', '34 Hood Avenue, Winnipeg, MB', 434900, 3, 3, 0, 'feras@ucalgary.ca', 1),</v>
+        <f t="shared" si="5"/>
+        <v>('202226895', '34 Hood Avenue, Winnipeg, MB', 434900, 3, 3, 'House', 'feras@ucalgary.ca', 1),</v>
       </c>
     </row>
     <row r="181" spans="1:10" x14ac:dyDescent="0.35">
@@ -6865,18 +7044,19 @@
       <c r="E181">
         <v>1</v>
       </c>
-      <c r="F181">
-        <v>0</v>
+      <c r="F181" t="str">
+        <f t="shared" si="4"/>
+        <v>House</v>
       </c>
       <c r="G181" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H181">
         <v>2</v>
       </c>
       <c r="J181" t="str">
-        <f t="shared" si="2"/>
-        <v>('202227006', '207 Edward Avenue, Winnipeg, MB', 319900, 3, 1, 0, 'feras@ucalgary.ca', 2),</v>
+        <f t="shared" si="5"/>
+        <v>('202227006', '207 Edward Avenue, Winnipeg, MB', 319900, 3, 1, 'House', 'feras@ucalgary.ca', 2),</v>
       </c>
     </row>
     <row r="182" spans="1:10" x14ac:dyDescent="0.35">
@@ -6895,18 +7075,19 @@
       <c r="E182">
         <v>3</v>
       </c>
-      <c r="F182">
-        <v>0</v>
+      <c r="F182" t="str">
+        <f t="shared" si="4"/>
+        <v>House</v>
       </c>
       <c r="G182" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H182">
         <v>3</v>
       </c>
       <c r="J182" t="str">
-        <f t="shared" si="2"/>
-        <v>('202226121', '58 Lindenwood Drive, Winnipeg, MB', 649900, 4, 3, 0, 'feras@ucalgary.ca', 3),</v>
+        <f t="shared" si="5"/>
+        <v>('202226121', '58 Lindenwood Drive, Winnipeg, MB', 649900, 4, 3, 'House', 'feras@ucalgary.ca', 3),</v>
       </c>
     </row>
     <row r="183" spans="1:10" x14ac:dyDescent="0.35">
@@ -6925,18 +7106,19 @@
       <c r="E183">
         <v>5</v>
       </c>
-      <c r="F183">
-        <v>0</v>
+      <c r="F183" t="str">
+        <f t="shared" si="4"/>
+        <v>House</v>
       </c>
       <c r="G183" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H183">
         <v>1</v>
       </c>
       <c r="J183" t="str">
-        <f t="shared" si="2"/>
-        <v>('202226911', '21 DISCOVERY Cove, Winnipeg, MB', 1490000, 6, 5, 0, 'feras@ucalgary.ca', 1),</v>
+        <f t="shared" si="5"/>
+        <v>('202226911', '21 DISCOVERY Cove, Winnipeg, MB', 1490000, 6, 5, 'House', 'feras@ucalgary.ca', 1),</v>
       </c>
     </row>
     <row r="184" spans="1:10" x14ac:dyDescent="0.35">
@@ -6955,18 +7137,19 @@
       <c r="E184">
         <v>2</v>
       </c>
-      <c r="F184">
-        <v>0</v>
+      <c r="F184" t="str">
+        <f t="shared" si="4"/>
+        <v>House</v>
       </c>
       <c r="G184" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H184">
         <v>2</v>
       </c>
       <c r="J184" t="str">
-        <f t="shared" si="2"/>
-        <v>('202226898', '251 Cullen Drive, Winnipeg, MB', 349900, 4, 2, 0, 'feras@ucalgary.ca', 2),</v>
+        <f t="shared" si="5"/>
+        <v>('202226898', '251 Cullen Drive, Winnipeg, MB', 349900, 4, 2, 'House', 'feras@ucalgary.ca', 2),</v>
       </c>
     </row>
     <row r="185" spans="1:10" x14ac:dyDescent="0.35">
@@ -6985,18 +7168,19 @@
       <c r="E185">
         <v>3</v>
       </c>
-      <c r="F185">
-        <v>0</v>
+      <c r="F185" t="str">
+        <f t="shared" si="4"/>
+        <v>House</v>
       </c>
       <c r="G185" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H185">
         <v>3</v>
       </c>
       <c r="J185" t="str">
-        <f t="shared" si="2"/>
-        <v>('202226907', '150 Nordstrom Drive, Winnipeg, MB', 499900, 3, 3, 0, 'feras@ucalgary.ca', 3),</v>
+        <f t="shared" si="5"/>
+        <v>('202226907', '150 Nordstrom Drive, Winnipeg, MB', 499900, 3, 3, 'House', 'feras@ucalgary.ca', 3),</v>
       </c>
     </row>
     <row r="186" spans="1:10" x14ac:dyDescent="0.35">
@@ -7015,18 +7199,19 @@
       <c r="E186">
         <v>1</v>
       </c>
-      <c r="F186">
-        <v>0</v>
+      <c r="F186" t="str">
+        <f t="shared" si="4"/>
+        <v>Condo</v>
       </c>
       <c r="G186" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H186">
         <v>1</v>
       </c>
       <c r="J186" t="str">
-        <f t="shared" si="2"/>
-        <v>('202226946', '789 Sherburn Street, Winnipeg, MB', 229900, 2, 1, 0, 'feras@ucalgary.ca', 1),</v>
+        <f t="shared" si="5"/>
+        <v>('202226946', '789 Sherburn Street, Winnipeg, MB', 229900, 2, 1, 'Condo', 'feras@ucalgary.ca', 1),</v>
       </c>
     </row>
     <row r="187" spans="1:10" x14ac:dyDescent="0.35">
@@ -7045,18 +7230,19 @@
       <c r="E187">
         <v>1</v>
       </c>
-      <c r="F187">
-        <v>0</v>
+      <c r="F187" t="str">
+        <f t="shared" si="4"/>
+        <v>House</v>
       </c>
       <c r="G187" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H187">
         <v>2</v>
       </c>
       <c r="J187" t="str">
-        <f t="shared" si="2"/>
-        <v>('202225745', '389 Beverley Street, Winnipeg, MB', 74900, 3, 1, 0, 'feras@ucalgary.ca', 2),</v>
+        <f t="shared" si="5"/>
+        <v>('202225745', '389 Beverley Street, Winnipeg, MB', 74900, 3, 1, 'House', 'feras@ucalgary.ca', 2),</v>
       </c>
     </row>
     <row r="188" spans="1:10" x14ac:dyDescent="0.35">
@@ -7075,18 +7261,19 @@
       <c r="E188">
         <v>3</v>
       </c>
-      <c r="F188">
-        <v>0</v>
+      <c r="F188" t="str">
+        <f t="shared" si="4"/>
+        <v>House</v>
       </c>
       <c r="G188" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H188">
         <v>3</v>
       </c>
       <c r="J188" t="str">
-        <f t="shared" si="2"/>
-        <v>('202225532', '11 Crocker Place, Winnipeg, MB', 899900, 4, 3, 0, 'feras@ucalgary.ca', 3),</v>
+        <f t="shared" si="5"/>
+        <v>('202225532', '11 Crocker Place, Winnipeg, MB', 899900, 4, 3, 'House', 'feras@ucalgary.ca', 3),</v>
       </c>
     </row>
   </sheetData>

</xml_diff>